<commit_message>
Added Washington Commanders name and logo
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C46B677-71D7-46A4-AD5A-FC43EF42771E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A986261F-2817-4FDD-86E9-C847EF2961C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>Washington</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Philadelphia</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>Patriots</t>
+  </si>
+  <si>
+    <t>Commanders</t>
   </si>
 </sst>
 </file>
@@ -983,66 +983,66 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
         <v>170</v>
-      </c>
-      <c r="B7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1066,33 +1066,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1150,42 +1150,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1205,21 +1205,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2">
         <v>0.875</v>
@@ -1247,7 +1247,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,7 +1278,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
@@ -1287,22 +1287,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1314,22 +1314,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1341,22 +1341,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1368,22 +1368,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1395,22 +1395,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>2022</v>
       </c>
       <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1422,22 +1422,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7">
         <v>2022</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1449,22 +1449,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8">
         <v>2022</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9">
         <v>2022</v>
@@ -1488,10 +1488,10 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
         <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1503,22 +1503,22 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10">
         <v>2022</v>
       </c>
       <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="D10" t="s">
-        <v>72</v>
-      </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1530,22 +1530,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11">
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1557,22 +1557,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12">
         <v>2022</v>
       </c>
       <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1584,22 +1584,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13">
         <v>2022</v>
       </c>
       <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1611,19 +1611,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>2022</v>
       </c>
       <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -1638,19 +1638,19 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15">
         <v>2022</v>
       </c>
       <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -1665,19 +1665,19 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16">
         <v>2022</v>
       </c>
       <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
         <v>41</v>
       </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17">
         <v>2022</v>
@@ -1704,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -1719,22 +1719,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18">
         <v>2022</v>
       </c>
       <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
         <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>45</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1746,22 +1746,22 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19">
         <v>2022</v>
       </c>
       <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
         <v>46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20">
         <v>2022</v>
@@ -1782,13 +1782,13 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21">
         <v>2022</v>
@@ -1815,7 +1815,7 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1827,22 +1827,22 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22">
         <v>2022</v>
       </c>
       <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>22</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23">
         <v>2022</v>
@@ -1869,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1881,22 +1881,22 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24">
         <v>2022</v>
       </c>
       <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>19</v>
-      </c>
-      <c r="D24" t="s">
-        <v>20</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25">
         <v>2022</v>
@@ -1917,40 +1917,40 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>('T24','2022','Washington','?','NFC','East',1),</v>
+        <v>('T24','2022','Washington','Commanders','NFC','East',1),</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26">
         <v>2022</v>
       </c>
       <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
         <v>65</v>
-      </c>
-      <c r="D26" t="s">
-        <v>66</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1962,22 +1962,22 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27">
         <v>2022</v>
       </c>
       <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
         <v>69</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1989,22 +1989,22 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28">
         <v>2022</v>
       </c>
       <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
         <v>67</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2016,22 +2016,22 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29">
         <v>2022</v>
       </c>
       <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
         <v>63</v>
-      </c>
-      <c r="D29" t="s">
-        <v>64</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -2043,16 +2043,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30">
         <v>2022</v>
       </c>
       <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
         <v>31</v>
-      </c>
-      <c r="D30" t="s">
-        <v>32</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31">
         <v>2022</v>
@@ -2097,16 +2097,16 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32">
         <v>2022</v>
       </c>
       <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
         <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>34</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -2124,16 +2124,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33">
         <v>2022</v>
       </c>
       <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
         <v>35</v>
-      </c>
-      <c r="D33" t="s">
-        <v>36</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -2183,45 +2183,45 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>115</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>116</v>
-      </c>
-      <c r="E2" t="s">
-        <v>117</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2262,58 +2262,58 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
         <v>125</v>
       </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
         <v>127</v>
       </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2341,42 +2341,42 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="3">
         <v>44449.013888888891</v>
@@ -2395,16 +2395,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="3">
         <v>44569.895833333336</v>
@@ -2423,16 +2423,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4" s="3">
         <v>44603.979166666664</v>
@@ -2451,16 +2451,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="3">
         <v>44636.833333333336</v>
@@ -2479,16 +2479,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>2022</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="3">
         <v>44680</v>
@@ -2510,10 +2510,10 @@
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2521,10 +2521,10 @@
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2532,10 +2532,10 @@
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2543,10 +2543,10 @@
         <v>2023</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2554,10 +2554,10 @@
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2582,30 +2582,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2626,39 +2626,39 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2682,21 +2682,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2722,30 +2722,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
         <v>157</v>
-      </c>
-      <c r="D2" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving onto populating searchable dropdown
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A986261F-2817-4FDD-86E9-C847EF2961C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B33169-AB5A-4F1C-A265-97E80AE724BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -1246,7 +1246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -2248,7 +2248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Started adding all tables
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B33169-AB5A-4F1C-A265-97E80AE724BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363B1B29-1CD8-4507-811C-B2761407FDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
     <sheet name="Teams" sheetId="1" r:id="rId2"/>
     <sheet name="Users" sheetId="2" r:id="rId3"/>
     <sheet name="Players" sheetId="3" r:id="rId4"/>
-    <sheet name="PredictionPeriodInfo" sheetId="4" r:id="rId5"/>
+    <sheet name="PredictionPeriods" sheetId="4" r:id="rId5"/>
     <sheet name="PeriodPredictions" sheetId="5" r:id="rId6"/>
-    <sheet name="PredictionsByWeek" sheetId="6" r:id="rId7"/>
+    <sheet name="WeekPredictions" sheetId="6" r:id="rId7"/>
     <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId8"/>
-    <sheet name="PrivateLeagueInfo" sheetId="8" r:id="rId9"/>
-    <sheet name="ScoringSettingsInfo" sheetId="10" r:id="rId10"/>
-    <sheet name="PrivateLeagueMembership" sheetId="11" r:id="rId11"/>
+    <sheet name="PrivateLeagues" sheetId="8" r:id="rId9"/>
+    <sheet name="ScoringSettings" sheetId="10" r:id="rId10"/>
+    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId11"/>
     <sheet name="UserScores" sheetId="12" r:id="rId12"/>
     <sheet name="SQL Commands" sheetId="13" r:id="rId13"/>
   </sheets>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="193">
   <si>
     <t>TeamID</t>
   </si>
@@ -375,18 +375,9 @@
     <t>EmailAddress</t>
   </si>
   <si>
-    <t>FavouriteTeam</t>
-  </si>
-  <si>
     <t>HashedPassword</t>
   </si>
   <si>
-    <t>Authenticated</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>UserCreated</t>
   </si>
   <si>
@@ -625,6 +616,18 @@
   </si>
   <si>
     <t>Commanders</t>
+  </si>
+  <si>
+    <t>FavouriteTeamID</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>IsAuthenticated</t>
+  </si>
+  <si>
+    <t>IsAdmin</t>
   </si>
 </sst>
 </file>
@@ -983,10 +986,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -994,55 +997,55 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1066,33 +1069,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1112,10 +1115,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1150,7 +1153,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -1161,7 +1164,7 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1169,7 +1172,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1177,7 +1180,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1185,7 +1188,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1205,21 +1208,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C2">
         <v>0.875</v>
@@ -1278,7 +1281,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
@@ -1458,7 +1461,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -1536,7 +1539,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -1917,7 +1920,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2163,10 +2166,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2177,11 +2180,12 @@
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -2192,49 +2196,55 @@
         <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
-      </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
         <v>44591.015905787041</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H3" s="3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2248,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2262,27 +2272,27 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
@@ -2290,13 +2300,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
@@ -2304,16 +2314,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2341,42 +2351,42 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E2" s="3">
         <v>44449.013888888891</v>
@@ -2395,16 +2405,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E3" s="3">
         <v>44569.895833333336</v>
@@ -2423,16 +2433,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E4" s="3">
         <v>44603.979166666664</v>
@@ -2451,16 +2461,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E5" s="3">
         <v>44636.833333333336</v>
@@ -2479,16 +2489,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B6">
         <v>2022</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E6" s="3">
         <v>44680</v>
@@ -2510,10 +2520,10 @@
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2521,10 +2531,10 @@
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2532,10 +2542,10 @@
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2543,10 +2553,10 @@
         <v>2023</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2554,10 +2564,10 @@
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2570,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2582,7 +2592,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -2591,21 +2601,21 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2626,10 +2636,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>105</v>
@@ -2638,27 +2648,27 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2682,7 +2692,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -2690,13 +2700,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2722,16 +2732,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2739,13 +2749,13 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More db work and getting all QBs
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363B1B29-1CD8-4507-811C-B2761407FDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D4DEB9-E3A7-48E3-8944-201016B4B394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
     <sheet name="Teams" sheetId="1" r:id="rId2"/>
-    <sheet name="Users" sheetId="2" r:id="rId3"/>
-    <sheet name="Players" sheetId="3" r:id="rId4"/>
+    <sheet name="Players" sheetId="3" r:id="rId3"/>
+    <sheet name="Users" sheetId="2" r:id="rId4"/>
     <sheet name="PredictionPeriods" sheetId="4" r:id="rId5"/>
     <sheet name="PeriodPredictions" sheetId="5" r:id="rId6"/>
     <sheet name="WeekPredictions" sheetId="6" r:id="rId7"/>
@@ -28,6 +28,7 @@
     <sheet name="SQL Commands" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$D$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Teams!$A$1:$G$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="367">
   <si>
     <t>TeamID</t>
   </si>
@@ -387,9 +388,6 @@
     <t>oliverdernie1@googlemail.com</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>####</t>
   </si>
   <si>
@@ -399,33 +397,9 @@
     <t>PlayerID</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>DefaultTeamID</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Brady</t>
-  </si>
-  <si>
-    <t>Kyler</t>
-  </si>
-  <si>
-    <t>Murray</t>
-  </si>
-  <si>
-    <t>Kyle</t>
-  </si>
-  <si>
-    <t>Trask</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -628,6 +602,555 @@
   </si>
   <si>
     <t>IsAdmin</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Tyler Huntley</t>
+  </si>
+  <si>
+    <t>Lamar Jackson</t>
+  </si>
+  <si>
+    <t>Case Keenum</t>
+  </si>
+  <si>
+    <t>Nick Mullens</t>
+  </si>
+  <si>
+    <t>Dwayne Haskins</t>
+  </si>
+  <si>
+    <t>Ben Roethlisberger</t>
+  </si>
+  <si>
+    <t>Mitchell Trubisky</t>
+  </si>
+  <si>
+    <t>Jacoby Brissett</t>
+  </si>
+  <si>
+    <t>Tua Tagovailoa</t>
+  </si>
+  <si>
+    <t>Brian Hoyer</t>
+  </si>
+  <si>
+    <t>Mac Jones</t>
+  </si>
+  <si>
+    <t>Jarrett Stidham</t>
+  </si>
+  <si>
+    <t>Joe Flacco</t>
+  </si>
+  <si>
+    <t>Zach Wilson</t>
+  </si>
+  <si>
+    <t>Davis Mills</t>
+  </si>
+  <si>
+    <t>Tyrod Taylor</t>
+  </si>
+  <si>
+    <t>Deshaun Watson</t>
+  </si>
+  <si>
+    <t>Sam Ehlinger</t>
+  </si>
+  <si>
+    <t>Carson Wentz</t>
+  </si>
+  <si>
+    <t>Trevor Lawrence</t>
+  </si>
+  <si>
+    <t>Ryan Tannehill</t>
+  </si>
+  <si>
+    <t>Logan Woodside</t>
+  </si>
+  <si>
+    <t>Drew Lock</t>
+  </si>
+  <si>
+    <t>Brett Rypien</t>
+  </si>
+  <si>
+    <t>Shane Buechele</t>
+  </si>
+  <si>
+    <t>Chad Henne</t>
+  </si>
+  <si>
+    <t>Patrick Mahomes</t>
+  </si>
+  <si>
+    <t>Derek Carr</t>
+  </si>
+  <si>
+    <t>Marcus Mariota</t>
+  </si>
+  <si>
+    <t>Chase Daniel</t>
+  </si>
+  <si>
+    <t>Justin Herbert</t>
+  </si>
+  <si>
+    <t>Easton Stick</t>
+  </si>
+  <si>
+    <t>Andy Dalton</t>
+  </si>
+  <si>
+    <t>Nick Foles</t>
+  </si>
+  <si>
+    <t>David Blough</t>
+  </si>
+  <si>
+    <t>Jared Goff</t>
+  </si>
+  <si>
+    <t>Jordan Love</t>
+  </si>
+  <si>
+    <t>Aaron Rodgers</t>
+  </si>
+  <si>
+    <t>Kirk Cousins</t>
+  </si>
+  <si>
+    <t>Kellen Mond</t>
+  </si>
+  <si>
+    <t>Dak Prescott</t>
+  </si>
+  <si>
+    <t>Cooper Rush</t>
+  </si>
+  <si>
+    <t>Jake Fromm</t>
+  </si>
+  <si>
+    <t>Mike Glennon</t>
+  </si>
+  <si>
+    <t>Jalen Hurts</t>
+  </si>
+  <si>
+    <t>Gardner Minshew</t>
+  </si>
+  <si>
+    <t>Reid Sinnett</t>
+  </si>
+  <si>
+    <t>Kyle Allen</t>
+  </si>
+  <si>
+    <t>Garrett Gilbert</t>
+  </si>
+  <si>
+    <t>Taylor Heinicke</t>
+  </si>
+  <si>
+    <t>Feleipe Franks</t>
+  </si>
+  <si>
+    <t>Josh Rosen</t>
+  </si>
+  <si>
+    <t>Sam Darnold</t>
+  </si>
+  <si>
+    <t>Cam Newton</t>
+  </si>
+  <si>
+    <t>P. J. Walker</t>
+  </si>
+  <si>
+    <t>Ian Book</t>
+  </si>
+  <si>
+    <t>Taysom Hill</t>
+  </si>
+  <si>
+    <t>Trevor Siemian</t>
+  </si>
+  <si>
+    <t>Tom Brady</t>
+  </si>
+  <si>
+    <t>Blaine Gabbert</t>
+  </si>
+  <si>
+    <t>Kyle Trask</t>
+  </si>
+  <si>
+    <t>Colt McCoy</t>
+  </si>
+  <si>
+    <t>Trace McSorley</t>
+  </si>
+  <si>
+    <t>Kyler Murray</t>
+  </si>
+  <si>
+    <t>Jimmy Garoppolo</t>
+  </si>
+  <si>
+    <t>Trey Lance</t>
+  </si>
+  <si>
+    <t>Jacob Eason</t>
+  </si>
+  <si>
+    <t>Geno Smith</t>
+  </si>
+  <si>
+    <t>Russell Wilson</t>
+  </si>
+  <si>
+    <t>Josh Johnson</t>
+  </si>
+  <si>
+    <t>Mason Rudolph</t>
+  </si>
+  <si>
+    <t>Josh Allen</t>
+  </si>
+  <si>
+    <t>Mike White</t>
+  </si>
+  <si>
+    <t>Tim Boyle</t>
+  </si>
+  <si>
+    <t>Sean Mannion</t>
+  </si>
+  <si>
+    <t>Matt Ryan</t>
+  </si>
+  <si>
+    <t>Brandon Allen</t>
+  </si>
+  <si>
+    <t>Joe Burrow</t>
+  </si>
+  <si>
+    <t>Baker Mayfield</t>
+  </si>
+  <si>
+    <t>Teddy Bridgewater</t>
+  </si>
+  <si>
+    <t>Justin Fields</t>
+  </si>
+  <si>
+    <t>Daniel Jones</t>
+  </si>
+  <si>
+    <t>Jameis Winston</t>
+  </si>
+  <si>
+    <t>Bryce Perkins</t>
+  </si>
+  <si>
+    <t>Matthew Stafford</t>
+  </si>
+  <si>
+    <t>John Wolford</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>P30</t>
+  </si>
+  <si>
+    <t>P31</t>
+  </si>
+  <si>
+    <t>P32</t>
+  </si>
+  <si>
+    <t>P33</t>
+  </si>
+  <si>
+    <t>P34</t>
+  </si>
+  <si>
+    <t>P35</t>
+  </si>
+  <si>
+    <t>P36</t>
+  </si>
+  <si>
+    <t>P37</t>
+  </si>
+  <si>
+    <t>P38</t>
+  </si>
+  <si>
+    <t>P39</t>
+  </si>
+  <si>
+    <t>P40</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>P42</t>
+  </si>
+  <si>
+    <t>P43</t>
+  </si>
+  <si>
+    <t>P44</t>
+  </si>
+  <si>
+    <t>P45</t>
+  </si>
+  <si>
+    <t>P46</t>
+  </si>
+  <si>
+    <t>P47</t>
+  </si>
+  <si>
+    <t>P48</t>
+  </si>
+  <si>
+    <t>P49</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>P51</t>
+  </si>
+  <si>
+    <t>P52</t>
+  </si>
+  <si>
+    <t>P53</t>
+  </si>
+  <si>
+    <t>P54</t>
+  </si>
+  <si>
+    <t>P55</t>
+  </si>
+  <si>
+    <t>P56</t>
+  </si>
+  <si>
+    <t>P57</t>
+  </si>
+  <si>
+    <t>P58</t>
+  </si>
+  <si>
+    <t>P59</t>
+  </si>
+  <si>
+    <t>P60</t>
+  </si>
+  <si>
+    <t>P61</t>
+  </si>
+  <si>
+    <t>P62</t>
+  </si>
+  <si>
+    <t>P63</t>
+  </si>
+  <si>
+    <t>P64</t>
+  </si>
+  <si>
+    <t>P65</t>
+  </si>
+  <si>
+    <t>P66</t>
+  </si>
+  <si>
+    <t>P67</t>
+  </si>
+  <si>
+    <t>P68</t>
+  </si>
+  <si>
+    <t>P69</t>
+  </si>
+  <si>
+    <t>P70</t>
+  </si>
+  <si>
+    <t>P71</t>
+  </si>
+  <si>
+    <t>P72</t>
+  </si>
+  <si>
+    <t>P73</t>
+  </si>
+  <si>
+    <t>P74</t>
+  </si>
+  <si>
+    <t>P75</t>
+  </si>
+  <si>
+    <t>P76</t>
+  </si>
+  <si>
+    <t>P77</t>
+  </si>
+  <si>
+    <t>P78</t>
+  </si>
+  <si>
+    <t>P79</t>
+  </si>
+  <si>
+    <t>P80</t>
+  </si>
+  <si>
+    <t>P81</t>
+  </si>
+  <si>
+    <t>P82</t>
+  </si>
+  <si>
+    <t>P83</t>
+  </si>
+  <si>
+    <t>P84</t>
+  </si>
+  <si>
+    <t>P85</t>
+  </si>
+  <si>
+    <t>P86</t>
+  </si>
+  <si>
+    <t>Kenny Pickett</t>
+  </si>
+  <si>
+    <t>Sam Howell</t>
+  </si>
+  <si>
+    <t>Malik Willis</t>
+  </si>
+  <si>
+    <t>Matt Corral</t>
+  </si>
+  <si>
+    <t>Carson Strong</t>
+  </si>
+  <si>
+    <t>Desmond Ridder</t>
+  </si>
+  <si>
+    <t>Bailey Zappe</t>
+  </si>
+  <si>
+    <t>P87</t>
+  </si>
+  <si>
+    <t>P88</t>
+  </si>
+  <si>
+    <t>P89</t>
+  </si>
+  <si>
+    <t>P90</t>
+  </si>
+  <si>
+    <t>P91</t>
+  </si>
+  <si>
+    <t>P92</t>
+  </si>
+  <si>
+    <t>P93</t>
   </si>
 </sst>
 </file>
@@ -986,10 +1509,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -997,55 +1520,55 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1069,33 +1592,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1115,10 +1638,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1153,7 +1676,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -1164,7 +1687,7 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1172,7 +1695,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1180,7 +1703,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1188,7 +1711,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1208,21 +1731,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2">
         <v>0.875</v>
@@ -1247,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,7 +1784,7 @@
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,14 +1804,14 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J1" t="str">
+        <v>134</v>
+      </c>
+      <c r="I1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
         <v>INSERT INTO the_qb_carousel.teams (TeamID,Season,Location,Nickname,Conference,Division,IsActive) VALUES</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1310,12 +1833,12 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="J2" t="str">
+      <c r="I2" t="str">
         <f>"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A2:F2)&amp;"',"&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
         <v>('T1','2022','Baltimore','Ravens','AFC','North',1),</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1337,12 +1860,12 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J33" si="0">"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A3:F3)&amp;"',"&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I33" si="0">"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A3:F3)&amp;"',"&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
         <v>('T2','2022','Cincinnati','Bengals','AFC','North',1),</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1364,12 +1887,12 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="J4" t="str">
+      <c r="I4" t="str">
         <f t="shared" si="0"/>
         <v>('T3','2022','Cleveland','Browns','AFC','North',1),</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1391,12 +1914,12 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="J5" t="str">
+      <c r="I5" t="str">
         <f t="shared" si="0"/>
         <v>('T4','2022','Pittsburgh','Steelers','AFC','North',1),</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1418,12 +1941,12 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="J6" t="str">
+      <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>('T5','2022','Buffalo','Bills','AFC','East',1),</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -1445,12 +1968,12 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="J7" t="str">
+      <c r="I7" t="str">
         <f t="shared" si="0"/>
         <v>('T6','2022','Miami','Dolphins','AFC','East',1),</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1461,7 +1984,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -1472,12 +1995,12 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="J8" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="0"/>
         <v>('T7','2022','New England','Patriots','AFC','East',1),</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -1499,12 +2022,12 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="J9" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>('T8','2022','New York','Jets','AFC','East',1),</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1526,12 +2049,12 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="J10" t="str">
+      <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>('T9','2022','Houston','Texans','AFC','South',1),</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -1539,7 +2062,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -1553,12 +2076,12 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="J11" t="str">
+      <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>('T10','2022','Indianapolis','Colts','AFC','South',1),</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -1580,12 +2103,12 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="J12" t="str">
+      <c r="I12" t="str">
         <f t="shared" si="0"/>
         <v>('T11','2022','Jacksonville','Jaguars','AFC','South',1),</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1607,12 +2130,12 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="J13" t="str">
+      <c r="I13" t="str">
         <f t="shared" si="0"/>
         <v>('T12','2022','Tennessee','Titans','AFC','South',1),</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -1634,12 +2157,12 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="J14" t="str">
+      <c r="I14" t="str">
         <f t="shared" si="0"/>
         <v>('T13','2022','Denver','Broncos','AFC','West',1),</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1661,12 +2184,12 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="J15" t="str">
+      <c r="I15" t="str">
         <f t="shared" si="0"/>
         <v>('T14','2022','Kansas City','Chiefs','AFC','West',1),</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -1688,12 +2211,12 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="J16" t="str">
+      <c r="I16" t="str">
         <f t="shared" si="0"/>
         <v>('T15','2022','Las Vegas','Raiders','AFC','West',1),</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1715,12 +2238,12 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="J17" t="str">
+      <c r="I17" t="str">
         <f t="shared" si="0"/>
         <v>('T16','2022','Los Angeles','Chargers','AFC','West',1),</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1742,12 +2265,12 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="J18" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="0"/>
         <v>('T17','2022','Chicago','Bears','NFC','North',1),</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1769,12 +2292,12 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="J19" t="str">
+      <c r="I19" t="str">
         <f t="shared" si="0"/>
         <v>('T18','2022','Detroit','Lions','NFC','North',1),</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1796,12 +2319,12 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="J20" t="str">
+      <c r="I20" t="str">
         <f t="shared" si="0"/>
         <v>('T19','2022','Green Bay','Packers','NFC','North',1),</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -1823,12 +2346,12 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="J21" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="0"/>
         <v>('T20','2022','Minnesota','Vikings','NFC','North',1),</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -1850,12 +2373,12 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="J22" t="str">
+      <c r="I22" t="str">
         <f t="shared" si="0"/>
         <v>('T21','2022','Dallas','Cowboys','NFC','East',1),</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -1877,12 +2400,12 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="J23" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="0"/>
         <v>('T22','2022','New York','Giants','NFC','East',1),</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1904,12 +2427,12 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="J24" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="0"/>
         <v>('T23','2022','Philadelphia','Eagles','NFC','East',1),</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1920,7 +2443,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -1931,12 +2454,12 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="J25" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="0"/>
         <v>('T24','2022','Washington','Commanders','NFC','East',1),</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -1958,12 +2481,12 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="J26" t="str">
+      <c r="I26" t="str">
         <f t="shared" si="0"/>
         <v>('T25','2022','Atlanta','Falcons','NFC','South',1),</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -1985,12 +2508,12 @@
       <c r="G27">
         <v>1</v>
       </c>
-      <c r="J27" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="0"/>
         <v>('T26','2022','Carolina','Panthers','NFC','South',1),</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -2012,12 +2535,12 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="J28" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="0"/>
         <v>('T27','2022','New Orleans','Saints','NFC','South',1),</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -2039,12 +2562,12 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="J29" t="str">
+      <c r="I29" t="str">
         <f t="shared" si="0"/>
         <v>('T28','2022','Tampa Bay','Buccaneers','NFC','South',1),</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -2066,12 +2589,12 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="J30" t="str">
+      <c r="I30" t="str">
         <f t="shared" si="0"/>
         <v>('T29','2022','Arizona','Cardinals','NFC','West',1),</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -2093,12 +2616,12 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="J31" t="str">
+      <c r="I31" t="str">
         <f t="shared" si="0"/>
         <v>('T30','2022','Los Angeles','Rams','NFC','West',1),</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -2120,12 +2643,12 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="J32" t="str">
+      <c r="I32" t="str">
         <f t="shared" si="0"/>
         <v>('T31','2022','San Francisco','49ers','NFC','West',1),</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -2147,7 +2670,7 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="J33" t="str">
+      <c r="I33" t="str">
         <f t="shared" si="0"/>
         <v>('T32','2022','Seattle','Seahawks','NFC','West',1)</v>
       </c>
@@ -2165,6 +2688,1544 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
+  <dimension ref="A1:F94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" t="str">
+        <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.teams (PlayerID,Name,DefaultTeamID,IsActive) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"('"&amp;A2&amp;"','"&amp;B2&amp;"',"&amp;IF(LEN(C2)&gt;0,"'"&amp;C2&amp;"'","NULL")&amp;","&amp;D2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <v>('P1','Aaron Rodgers','T19',1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">"('"&amp;A3&amp;"','"&amp;B3&amp;"',"&amp;IF(LEN(C3)&gt;0,"'"&amp;C3&amp;"'","NULL")&amp;","&amp;D3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <v>('P2','Andy Dalton',NULL,1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>('P3','Baker Mayfield','T3',1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>('P4','Ben Roethlisberger','T4',1),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>('P5','Blaine Gabbert',NULL,1),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>('P6','Brandon Allen',NULL,1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>('P7','Brett Rypien',NULL,1),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>('P8','Brian Hoyer',NULL,1),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>('P9','Bryce Perkins',NULL,1),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>('P10','Cam Newton',NULL,1),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>('P11','Carson Wentz','T10',1),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>('P12','Case Keenum',NULL,1),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>('P13','Chad Henne',NULL,1),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>('P14','Chase Daniel',NULL,1),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>281</v>
+      </c>
+      <c r="B16" t="s">
+        <v>246</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>('P15','Colt McCoy',NULL,1),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>('P16','Cooper Rush',NULL,1),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>283</v>
+      </c>
+      <c r="B18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>('P17','Dak Prescott','T21',1),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>284</v>
+      </c>
+      <c r="B19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>('P18','Daniel Jones','T22',1),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B20" t="s">
+        <v>219</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>('P19','David Blough',NULL,1),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>286</v>
+      </c>
+      <c r="B21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>('P20','Davis Mills','T9',1),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>287</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>('P21','Derek Carr','T15',1),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>('P22','Deshaun Watson',NULL,1),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>289</v>
+      </c>
+      <c r="B24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>('P23','Drew Lock',NULL,1),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B25" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>('P24','Dwayne Haskins',NULL,1),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>('P25','Easton Stick',NULL,1),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>292</v>
+      </c>
+      <c r="B27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>('P26','Feleipe Franks',NULL,1),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>293</v>
+      </c>
+      <c r="B28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>('P27','Gardner Minshew',NULL,1),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>('P28','Garrett Gilbert',NULL,1),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>295</v>
+      </c>
+      <c r="B30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>('P29','Geno Smith',NULL,1),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>296</v>
+      </c>
+      <c r="B31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>('P30','Ian Book',NULL,1),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>297</v>
+      </c>
+      <c r="B32" t="s">
+        <v>251</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>('P31','Jacob Eason',NULL,1),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>298</v>
+      </c>
+      <c r="B33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>('P32','Jacoby Brissett',NULL,1),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>299</v>
+      </c>
+      <c r="B34" t="s">
+        <v>227</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>('P33','Jake Fromm',NULL,1),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>300</v>
+      </c>
+      <c r="B35" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>('P34','Jalen Hurts','T23',1),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" t="s">
+        <v>267</v>
+      </c>
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>('P35','Jameis Winston','T27',1),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>302</v>
+      </c>
+      <c r="B37" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>('P36','Jared Goff','T18',1),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>303</v>
+      </c>
+      <c r="B38" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>('P37','Jarrett Stidham',NULL,1),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>304</v>
+      </c>
+      <c r="B39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>('P38','Jimmy Garoppolo','T31',1),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B40" t="s">
+        <v>262</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>('P39','Joe Burrow','T2',1),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>306</v>
+      </c>
+      <c r="B41" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>('P40','Joe Flacco',NULL,1),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>307</v>
+      </c>
+      <c r="B42" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>('P41','John Wolford',NULL,1),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>308</v>
+      </c>
+      <c r="B43" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>('P42','Jordan Love',NULL,1),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>309</v>
+      </c>
+      <c r="B44" t="s">
+        <v>256</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>('P43','Josh Allen',NULL,1),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>310</v>
+      </c>
+      <c r="B45" t="s">
+        <v>254</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>('P44','Josh Johnson',NULL,1),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>311</v>
+      </c>
+      <c r="B46" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>('P45','Josh Rosen',NULL,1),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>312</v>
+      </c>
+      <c r="B47" t="s">
+        <v>265</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>('P46','Justin Fields','T17',1),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>313</v>
+      </c>
+      <c r="B48" t="s">
+        <v>215</v>
+      </c>
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>('P47','Justin Herbert','T16',1),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>314</v>
+      </c>
+      <c r="B49" t="s">
+        <v>224</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>('P48','Kellen Mond',NULL,1),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>315</v>
+      </c>
+      <c r="B50" t="s">
+        <v>223</v>
+      </c>
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>('P49','Kirk Cousins','T20',1),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" t="s">
+        <v>232</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>('P50','Kyle Allen',NULL,1),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>317</v>
+      </c>
+      <c r="B52" t="s">
+        <v>245</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>('P51','Kyle Trask',NULL,1),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>318</v>
+      </c>
+      <c r="B53" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>('P52','Kyler Murray','T29',1),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>319</v>
+      </c>
+      <c r="B54" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>('P53','Lamar Jackson','T1',1),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>320</v>
+      </c>
+      <c r="B55" t="s">
+        <v>206</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>('P54','Logan Woodside',NULL,1),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>321</v>
+      </c>
+      <c r="B56" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>('P55','Mac Jones','T7',1),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>322</v>
+      </c>
+      <c r="B57" t="s">
+        <v>213</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>('P56','Marcus Mariota',NULL,1),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>323</v>
+      </c>
+      <c r="B58" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>('P57','Mason Rudolph',NULL,1),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>('P58','Matt Ryan','T25',1),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>325</v>
+      </c>
+      <c r="B60" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>('P59','Matthew Stafford','T30',1),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>326</v>
+      </c>
+      <c r="B61" t="s">
+        <v>228</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>('P60','Mike Glennon',NULL,1),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>327</v>
+      </c>
+      <c r="B62" t="s">
+        <v>257</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>('P61','Mike White',NULL,1),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>328</v>
+      </c>
+      <c r="B63" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>('P62','Mitchell Trubisky','T5',1),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>329</v>
+      </c>
+      <c r="B64" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>('P63','Nick Foles',NULL,1),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>330</v>
+      </c>
+      <c r="B65" t="s">
+        <v>188</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>('P64','Nick Mullens',NULL,1),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>331</v>
+      </c>
+      <c r="B66" t="s">
+        <v>239</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>('P65','P. J. Walker',NULL,1),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>332</v>
+      </c>
+      <c r="B67" t="s">
+        <v>211</v>
+      </c>
+      <c r="C67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F94" si="1">"('"&amp;A67&amp;"','"&amp;B67&amp;"',"&amp;IF(LEN(C67)&gt;0,"'"&amp;C67&amp;"'","NULL")&amp;","&amp;D67&amp;")"&amp;IF(LEN(A68)&gt;0,",","")</f>
+        <v>('P66','Patrick Mahomes','T14',1),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>333</v>
+      </c>
+      <c r="B68" t="s">
+        <v>231</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="1"/>
+        <v>('P67','Reid Sinnett',NULL,1),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>334</v>
+      </c>
+      <c r="B69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="1"/>
+        <v>('P68','Russell Wilson','T32',1),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>335</v>
+      </c>
+      <c r="B70" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="1"/>
+        <v>('P69','Ryan Tannehill','T12',1),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>336</v>
+      </c>
+      <c r="B71" t="s">
+        <v>237</v>
+      </c>
+      <c r="C71" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="1"/>
+        <v>('P70','Sam Darnold','T26',1),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>337</v>
+      </c>
+      <c r="B72" t="s">
+        <v>202</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="1"/>
+        <v>('P71','Sam Ehlinger',NULL,1),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>338</v>
+      </c>
+      <c r="B73" t="s">
+        <v>259</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="1"/>
+        <v>('P72','Sean Mannion',NULL,1),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>339</v>
+      </c>
+      <c r="B74" t="s">
+        <v>209</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="1"/>
+        <v>('P73','Shane Buechele',NULL,1),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>340</v>
+      </c>
+      <c r="B75" t="s">
+        <v>234</v>
+      </c>
+      <c r="C75" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="1"/>
+        <v>('P74','Taylor Heinicke','T24',1),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>341</v>
+      </c>
+      <c r="B76" t="s">
+        <v>241</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="1"/>
+        <v>('P75','Taysom Hill',NULL,1),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>342</v>
+      </c>
+      <c r="B77" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" t="s">
+        <v>85</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="1"/>
+        <v>('P76','Teddy Bridgewater','T13',1),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>343</v>
+      </c>
+      <c r="B78" t="s">
+        <v>258</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="1"/>
+        <v>('P77','Tim Boyle',NULL,1),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>344</v>
+      </c>
+      <c r="B79" t="s">
+        <v>243</v>
+      </c>
+      <c r="C79" t="s">
+        <v>100</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="1"/>
+        <v>('P78','Tom Brady','T28',1),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>345</v>
+      </c>
+      <c r="B80" t="s">
+        <v>247</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="1"/>
+        <v>('P79','Trace McSorley',NULL,1),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>346</v>
+      </c>
+      <c r="B81" t="s">
+        <v>204</v>
+      </c>
+      <c r="C81" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="1"/>
+        <v>('P80','Trevor Lawrence','T11',1),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>347</v>
+      </c>
+      <c r="B82" t="s">
+        <v>242</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="1"/>
+        <v>('P81','Trevor Siemian',NULL,1),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>348</v>
+      </c>
+      <c r="B83" t="s">
+        <v>250</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="1"/>
+        <v>('P82','Trey Lance',NULL,1),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>349</v>
+      </c>
+      <c r="B84" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" t="s">
+        <v>78</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="1"/>
+        <v>('P83','Tua Tagovailoa','T6',1),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>350</v>
+      </c>
+      <c r="B85" t="s">
+        <v>185</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="F85" t="str">
+        <f t="shared" si="1"/>
+        <v>('P84','Tyler Huntley',NULL,1),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>351</v>
+      </c>
+      <c r="B86" t="s">
+        <v>200</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" si="1"/>
+        <v>('P85','Tyrod Taylor',NULL,1),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>352</v>
+      </c>
+      <c r="B87" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" t="s">
+        <v>80</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="F87" t="str">
+        <f t="shared" si="1"/>
+        <v>('P86','Zach Wilson','T8',1),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>360</v>
+      </c>
+      <c r="B88" t="s">
+        <v>359</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="F88" t="str">
+        <f t="shared" si="1"/>
+        <v>('P87','Bailey Zappe',NULL,1),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>361</v>
+      </c>
+      <c r="B89" t="s">
+        <v>357</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="F89" t="str">
+        <f t="shared" si="1"/>
+        <v>('P88','Carson Strong',NULL,1),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>362</v>
+      </c>
+      <c r="B90" t="s">
+        <v>358</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="F90" t="str">
+        <f t="shared" si="1"/>
+        <v>('P89','Desmond Ridder',NULL,1),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>363</v>
+      </c>
+      <c r="B91" t="s">
+        <v>353</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="F91" t="str">
+        <f t="shared" si="1"/>
+        <v>('P90','Kenny Pickett',NULL,1),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>364</v>
+      </c>
+      <c r="B92" t="s">
+        <v>355</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="F92" t="str">
+        <f t="shared" si="1"/>
+        <v>('P91','Malik Willis',NULL,1),</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>365</v>
+      </c>
+      <c r="B93" t="s">
+        <v>356</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="F93" t="str">
+        <f t="shared" si="1"/>
+        <v>('P92','Matt Corral',NULL,1),</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>366</v>
+      </c>
+      <c r="B94" t="s">
+        <v>354</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="F94" t="str">
+        <f t="shared" si="1"/>
+        <v>('P93','Sam Howell',NULL,1)</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D87" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D87">
+      <sortCondition ref="B1:B87"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B88:B94">
+    <sortCondition ref="B88:B94"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2196,19 +4257,19 @@
         <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>109</v>
@@ -2216,7 +4277,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
         <v>110</v>
@@ -2225,10 +4286,10 @@
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2250,83 +4311,6 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F1298F94-5BF1-4CAB-88DA-9474098335DF}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2351,42 +4335,42 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E2" s="3">
         <v>44449.013888888891</v>
@@ -2405,16 +4389,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E3" s="3">
         <v>44569.895833333336</v>
@@ -2433,16 +4417,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E4" s="3">
         <v>44603.979166666664</v>
@@ -2461,16 +4445,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E5" s="3">
         <v>44636.833333333336</v>
@@ -2489,16 +4473,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B6">
         <v>2022</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E6" s="3">
         <v>44680</v>
@@ -2520,10 +4504,10 @@
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2531,10 +4515,10 @@
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2542,10 +4526,10 @@
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2553,10 +4537,10 @@
         <v>2023</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2564,10 +4548,10 @@
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2580,7 +4564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -2592,7 +4576,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -2601,21 +4585,21 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2636,10 +4620,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>105</v>
@@ -2648,27 +4632,27 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2692,7 +4676,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>105</v>
@@ -2700,13 +4684,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2732,16 +4716,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2749,13 +4733,13 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Models done, I think
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D4DEB9-E3A7-48E3-8944-201016B4B394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C83CC39-3B37-4BAA-AD30-8A47FD3E7709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="371">
   <si>
     <t>TeamID</t>
   </si>
@@ -481,12 +481,6 @@
     <t>OwnerUserID</t>
   </si>
   <si>
-    <t>LeagueUUID</t>
-  </si>
-  <si>
-    <t>UUID()</t>
-  </si>
-  <si>
     <t>SS1</t>
   </si>
   <si>
@@ -1151,13 +1145,31 @@
   </si>
   <si>
     <t>P93</t>
+  </si>
+  <si>
+    <t>SeasonPeriodID</t>
+  </si>
+  <si>
+    <t>PP6</t>
+  </si>
+  <si>
+    <t>PP7</t>
+  </si>
+  <si>
+    <t>PP8</t>
+  </si>
+  <si>
+    <t>PP9</t>
+  </si>
+  <si>
+    <t>PP10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1187,6 +1199,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1209,12 +1229,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1509,10 +1530,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1520,55 +1541,55 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1580,9 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1591,34 +1610,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1638,10 +1657,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1669,16 +1688,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1695,7 +1714,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1703,7 +1722,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1711,7 +1730,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1723,21 +1742,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1772,9 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1785,7 +1805,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1984,7 +2004,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -2062,7 +2082,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -2443,7 +2463,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2691,9 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2703,11 +2721,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>115</v>
@@ -2725,7 +2743,7 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
@@ -2743,7 +2761,7 @@
         <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2758,7 +2776,7 @@
         <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
@@ -2773,10 +2791,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -2791,10 +2809,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2806,10 +2824,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2821,10 +2839,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2836,10 +2854,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2851,10 +2869,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2869,7 +2887,7 @@
         <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2881,10 +2899,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -2899,10 +2917,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2914,10 +2932,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2929,10 +2947,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2944,10 +2962,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2959,10 +2977,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2974,10 +2992,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
@@ -2992,10 +3010,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
         <v>94</v>
@@ -3010,10 +3028,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3025,10 +3043,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C21" t="s">
         <v>81</v>
@@ -3043,10 +3061,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -3061,10 +3079,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3076,10 +3094,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3091,10 +3109,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3106,10 +3124,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3121,10 +3139,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3136,10 +3154,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3151,10 +3169,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3166,10 +3184,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B30" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3181,10 +3199,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B31" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3196,10 +3214,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3211,10 +3229,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3226,10 +3244,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3241,10 +3259,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C35" t="s">
         <v>95</v>
@@ -3259,10 +3277,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B36" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C36" t="s">
         <v>99</v>
@@ -3277,10 +3295,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C37" t="s">
         <v>90</v>
@@ -3295,10 +3313,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3310,10 +3328,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C39" t="s">
         <v>103</v>
@@ -3328,10 +3346,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B40" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s">
         <v>74</v>
@@ -3346,10 +3364,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3361,10 +3379,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B42" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3376,10 +3394,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3391,10 +3409,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -3406,10 +3424,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B45" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3421,10 +3439,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3436,10 +3454,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C47" t="s">
         <v>89</v>
@@ -3454,10 +3472,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B48" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -3472,10 +3490,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3487,10 +3505,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C50" t="s">
         <v>92</v>
@@ -3505,10 +3523,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B51" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3520,10 +3538,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B52" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3535,10 +3553,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B53" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C53" t="s">
         <v>101</v>
@@ -3553,10 +3571,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C54" t="s">
         <v>72</v>
@@ -3571,10 +3589,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B55" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3586,10 +3604,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C56" t="s">
         <v>79</v>
@@ -3604,10 +3622,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B57" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3619,10 +3637,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B58" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3634,10 +3652,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B59" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -3652,10 +3670,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B60" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
@@ -3670,10 +3688,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B61" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -3685,10 +3703,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B62" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3700,10 +3718,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C63" t="s">
         <v>77</v>
@@ -3718,10 +3736,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3733,10 +3751,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -3748,10 +3766,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -3763,10 +3781,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
@@ -3781,10 +3799,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B68" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -3796,10 +3814,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B69" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C69" t="s">
         <v>104</v>
@@ -3814,10 +3832,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C70" t="s">
         <v>84</v>
@@ -3832,10 +3850,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B71" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C71" t="s">
         <v>98</v>
@@ -3850,10 +3868,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -3865,10 +3883,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B73" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -3880,10 +3898,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -3895,10 +3913,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
@@ -3913,10 +3931,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B76" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -3928,10 +3946,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B77" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C77" t="s">
         <v>85</v>
@@ -3946,10 +3964,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B78" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -3961,10 +3979,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C79" t="s">
         <v>100</v>
@@ -3979,10 +3997,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -3994,10 +4012,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C81" t="s">
         <v>83</v>
@@ -4012,10 +4030,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B82" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4027,10 +4045,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B83" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4042,10 +4060,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B84" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C84" t="s">
         <v>78</v>
@@ -4060,10 +4078,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B85" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4075,10 +4093,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B86" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -4090,10 +4108,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B87" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C87" t="s">
         <v>80</v>
@@ -4108,10 +4126,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B88" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4123,10 +4141,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B89" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4138,10 +4156,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B90" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4153,10 +4171,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B91" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4168,10 +4186,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B92" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4183,10 +4201,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B93" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4198,10 +4216,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B94" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4229,9 +4247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4247,7 +4263,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4257,19 +4273,19 @@
         <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>109</v>
@@ -4286,7 +4302,7 @@
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>112</v>
@@ -4319,9 +4335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4334,14 +4348,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>365</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>122</v>
@@ -4367,7 +4381,7 @@
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
         <v>123</v>
@@ -4395,7 +4409,7 @@
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>124</v>
@@ -4423,7 +4437,7 @@
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
         <v>126</v>
@@ -4451,7 +4465,7 @@
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
         <v>127</v>
@@ -4479,10 +4493,10 @@
         <v>2022</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E6" s="3">
         <v>44680</v>
@@ -4500,58 +4514,73 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>366</v>
+      </c>
       <c r="B7">
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>367</v>
+      </c>
       <c r="B8">
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>368</v>
+      </c>
       <c r="B9">
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>369</v>
+      </c>
       <c r="B10">
         <v>2023</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>370</v>
+      </c>
       <c r="B11">
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4565,7 +4594,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4575,13 +4604,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -4611,24 +4640,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF7E11E-B54A-4612-A949-04C2EF515915}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -4665,7 +4700,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4675,10 +4710,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -4700,35 +4735,29 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -4736,10 +4765,7 @@
         <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Teams and Players APIs working
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C83CC39-3B37-4BAA-AD30-8A47FD3E7709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E5361B-E7AD-4F5A-B9B7-F8692A5780E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -47,6 +47,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1742,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2709,9 +2731,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2720,7 +2744,7 @@
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -2733,12 +2757,12 @@
       <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F1" t="str">
-        <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
-        <v>INSERT INTO the_qb_carousel.teams (PlayerID,Name,DefaultTeamID,IsActive) VALUES</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" t="str" cm="1">
+        <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.Players(PlayerID,Name,DefaultTeamID,IsActive) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -2756,7 +2780,7 @@
         <v>('P1','Aaron Rodgers','T19',1),</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -2771,7 +2795,7 @@
         <v>('P2','Andy Dalton',NULL,1),</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -2788,8 +2812,12 @@
         <f t="shared" si="0"/>
         <v>('P3','Baker Mayfield','T3',1),</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K4" t="str" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
+        <v>Players</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>269</v>
       </c>
@@ -2807,7 +2835,7 @@
         <v>('P4','Ben Roethlisberger','T4',1),</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>270</v>
       </c>
@@ -2822,7 +2850,7 @@
         <v>('P5','Blaine Gabbert',NULL,1),</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>271</v>
       </c>
@@ -2837,7 +2865,7 @@
         <v>('P6','Brandon Allen',NULL,1),</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -2852,7 +2880,7 @@
         <v>('P7','Brett Rypien',NULL,1),</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>273</v>
       </c>
@@ -2867,7 +2895,7 @@
         <v>('P8','Brian Hoyer',NULL,1),</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -2882,7 +2910,7 @@
         <v>('P9','Bryce Perkins',NULL,1),</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -2897,7 +2925,7 @@
         <v>('P10','Cam Newton',NULL,1),</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>275</v>
       </c>
@@ -2915,7 +2943,7 @@
         <v>('P11','Carson Wentz','T10',1),</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>276</v>
       </c>
@@ -2930,7 +2958,7 @@
         <v>('P12','Case Keenum',NULL,1),</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>277</v>
       </c>
@@ -2945,7 +2973,7 @@
         <v>('P13','Chad Henne',NULL,1),</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>278</v>
       </c>
@@ -2960,7 +2988,7 @@
         <v>('P14','Chase Daniel',NULL,1),</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>279</v>
       </c>
@@ -4341,7 +4369,7 @@
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
qb-predictions layout complete, 'save' and 'suggestions' to go
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E5361B-E7AD-4F5A-B9B7-F8692A5780E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B92A6C-15C1-49B2-921C-A0D223468490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,20 +16,21 @@
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
     <sheet name="Teams" sheetId="1" r:id="rId2"/>
     <sheet name="Players" sheetId="3" r:id="rId3"/>
-    <sheet name="Users" sheetId="2" r:id="rId4"/>
-    <sheet name="PredictionPeriods" sheetId="4" r:id="rId5"/>
-    <sheet name="PeriodPredictions" sheetId="5" r:id="rId6"/>
-    <sheet name="WeekPredictions" sheetId="6" r:id="rId7"/>
-    <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId8"/>
-    <sheet name="PrivateLeagues" sheetId="8" r:id="rId9"/>
-    <sheet name="ScoringSettings" sheetId="10" r:id="rId10"/>
-    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId11"/>
-    <sheet name="UserScores" sheetId="12" r:id="rId12"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId13"/>
+    <sheet name="Conferences" sheetId="14" r:id="rId4"/>
+    <sheet name="Users" sheetId="2" r:id="rId5"/>
+    <sheet name="PredictionPeriods" sheetId="4" r:id="rId6"/>
+    <sheet name="PeriodPredictions" sheetId="5" r:id="rId7"/>
+    <sheet name="WeekPredictions" sheetId="6" r:id="rId8"/>
+    <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId9"/>
+    <sheet name="PrivateLeagues" sheetId="8" r:id="rId10"/>
+    <sheet name="ScoringSettings" sheetId="10" r:id="rId11"/>
+    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId12"/>
+    <sheet name="UserScores" sheetId="12" r:id="rId13"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$D$87</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Teams!$A$1:$G$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Teams!$A$1:$I$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="379">
   <si>
     <t>TeamID</t>
   </si>
@@ -1185,6 +1186,30 @@
   </si>
   <si>
     <t>PP10</t>
+  </si>
+  <si>
+    <t>GridColumn</t>
+  </si>
+  <si>
+    <t>GridRow</t>
+  </si>
+  <si>
+    <t>ConferenceID</t>
+  </si>
+  <si>
+    <t>GridRowStart</t>
+  </si>
+  <si>
+    <t>GridRowEnd</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
 </sst>
 </file>
@@ -1539,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD2AB4C-1FDF-40BE-911A-52427E1B6DC0}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,12 +1639,60 @@
         <v>157</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1705,7 +1778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6954B5E2-894C-437E-8E51-B1D29E513C99}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1760,7 +1833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1800,7 +1873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1814,9 +1887,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1824,9 +1899,11 @@
     <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1848,12 +1925,18 @@
       <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I1" t="str">
-        <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
-        <v>INSERT INTO the_qb_carousel.teams (TeamID,Season,Location,Nickname,Conference,Division,IsActive) VALUES</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K1" t="str">
+        <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:I1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.teams (TeamID,Season,Location,Nickname,Conference,Division,IsActive,GridColumn,GridRow) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1875,12 +1958,18 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2" t="str">
-        <f>"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A2:F2)&amp;"',"&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
-        <v>('T1','2022','Baltimore','Ravens','AFC','North',1),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A2:F2)&amp;"',"&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <v>('T1','2022','Baltimore','Ravens','AFC','North',1,2,2),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1902,12 +1991,18 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I33" si="0">"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A3:F3)&amp;"',"&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
-        <v>('T2','2022','Cincinnati','Bengals','AFC','North',1),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K33" si="0">"('"&amp;_xlfn.TEXTJOIN("','",FALSE,A3:F3)&amp;"',"&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <v>('T2','2022','Cincinnati','Bengals','AFC','North',1,2,3),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1929,12 +2024,18 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>('T3','2022','Cleveland','Browns','AFC','North',1),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>('T3','2022','Cleveland','Browns','AFC','North',1,2,4),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1956,12 +2057,18 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>('T4','2022','Pittsburgh','Steelers','AFC','North',1),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>('T4','2022','Pittsburgh','Steelers','AFC','North',1,2,5),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1983,12 +2090,18 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>('T5','2022','Buffalo','Bills','AFC','East',1),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>('T5','2022','Buffalo','Bills','AFC','East',1,3,2),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -2010,12 +2123,18 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>('T6','2022','Miami','Dolphins','AFC','East',1),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>('T6','2022','Miami','Dolphins','AFC','East',1,3,3),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -2037,12 +2156,18 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>('T7','2022','New England','Patriots','AFC','East',1),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>('T7','2022','New England','Patriots','AFC','East',1,3,4),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2064,12 +2189,18 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>('T8','2022','New York','Jets','AFC','East',1),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>('T8','2022','New York','Jets','AFC','East',1,3,5),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2091,12 +2222,18 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>('T9','2022','Houston','Texans','AFC','South',1),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>('T9','2022','Houston','Texans','AFC','South',1,4,2),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2118,12 +2255,18 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>('T10','2022','Indianapolis','Colts','AFC','South',1),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>('T10','2022','Indianapolis','Colts','AFC','South',1,4,3),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -2145,12 +2288,18 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>('T11','2022','Jacksonville','Jaguars','AFC','South',1),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>('T11','2022','Jacksonville','Jaguars','AFC','South',1,4,4),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -2172,12 +2321,18 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>('T12','2022','Tennessee','Titans','AFC','South',1),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>('T12','2022','Tennessee','Titans','AFC','South',1,4,5),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -2199,12 +2354,18 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>('T13','2022','Denver','Broncos','AFC','West',1),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>('T13','2022','Denver','Broncos','AFC','West',1,5,2),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -2226,12 +2387,18 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>('T14','2022','Kansas City','Chiefs','AFC','West',1),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>('T14','2022','Kansas City','Chiefs','AFC','West',1,5,3),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -2253,12 +2420,18 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>('T15','2022','Las Vegas','Raiders','AFC','West',1),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>('T15','2022','Las Vegas','Raiders','AFC','West',1,5,4),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -2280,12 +2453,18 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>('T16','2022','Los Angeles','Chargers','AFC','West',1),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>('T16','2022','Los Angeles','Chargers','AFC','West',1,5,5),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -2307,12 +2486,18 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>('T17','2022','Chicago','Bears','NFC','North',1),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>('T17','2022','Chicago','Bears','NFC','North',1,2,6),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -2334,12 +2519,18 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>('T18','2022','Detroit','Lions','NFC','North',1),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>('T18','2022','Detroit','Lions','NFC','North',1,2,7),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2361,12 +2552,18 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>('T19','2022','Green Bay','Packers','NFC','North',1),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>('T19','2022','Green Bay','Packers','NFC','North',1,2,8),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2388,12 +2585,18 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>('T20','2022','Minnesota','Vikings','NFC','North',1),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>('T20','2022','Minnesota','Vikings','NFC','North',1,2,9),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2415,12 +2618,18 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>('T21','2022','Dallas','Cowboys','NFC','East',1),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>('T21','2022','Dallas','Cowboys','NFC','East',1,3,6),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -2442,12 +2651,18 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>('T22','2022','New York','Giants','NFC','East',1),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>('T22','2022','New York','Giants','NFC','East',1,3,7),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -2469,12 +2684,18 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>('T23','2022','Philadelphia','Eagles','NFC','East',1),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>8</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>('T23','2022','Philadelphia','Eagles','NFC','East',1,3,8),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2496,12 +2717,18 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>('T24','2022','Washington','Commanders','NFC','East',1),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>('T24','2022','Washington','Commanders','NFC','East',1,3,9),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -2523,12 +2750,18 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>('T25','2022','Atlanta','Falcons','NFC','South',1),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>('T25','2022','Atlanta','Falcons','NFC','South',1,4,6),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -2550,12 +2783,18 @@
       <c r="G27">
         <v>1</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>('T26','2022','Carolina','Panthers','NFC','South',1),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>('T26','2022','Carolina','Panthers','NFC','South',1,4,7),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -2577,12 +2816,18 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>('T27','2022','New Orleans','Saints','NFC','South',1),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>('T27','2022','New Orleans','Saints','NFC','South',1,4,8),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -2604,12 +2849,18 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>('T28','2022','Tampa Bay','Buccaneers','NFC','South',1),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>('T28','2022','Tampa Bay','Buccaneers','NFC','South',1,4,9),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -2631,12 +2882,18 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>('T29','2022','Arizona','Cardinals','NFC','West',1),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>('T29','2022','Arizona','Cardinals','NFC','West',1,5,6),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -2658,12 +2915,18 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="I31" t="str">
-        <f t="shared" si="0"/>
-        <v>('T30','2022','Los Angeles','Rams','NFC','West',1),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>7</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>('T30','2022','Los Angeles','Rams','NFC','West',1,5,7),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -2685,12 +2948,18 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="I32" t="str">
-        <f t="shared" si="0"/>
-        <v>('T31','2022','San Francisco','49ers','NFC','West',1),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>('T31','2022','San Francisco','49ers','NFC','West',1,5,8),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -2712,13 +2981,20 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="I33" t="str">
-        <f t="shared" si="0"/>
-        <v>('T32','2022','Seattle','Seahawks','NFC','West',1)</v>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33">
+        <v>9</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>('T32','2022','Seattle','Seahawks','NFC','West',1,5,9)</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G33">
+  <autoFilter ref="A1:I33" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I33">
     <sortCondition ref="E2:E33"/>
     <sortCondition ref="F2:F33" customList="North,East,South,West"/>
     <sortCondition ref="C2:C33"/>
@@ -2733,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3442,12 +3718,15 @@
       <c r="B44" t="s">
         <v>254</v>
       </c>
+      <c r="C44" t="s">
+        <v>77</v>
+      </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>('P43','Josh Allen',NULL,1),</v>
+        <v>('P43','Josh Allen','T5',1),</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3751,15 +4030,12 @@
       <c r="B63" t="s">
         <v>189</v>
       </c>
-      <c r="C63" t="s">
-        <v>77</v>
-      </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>('P62','Mitchell Trubisky','T5',1),</v>
+        <v>('P62','Mitchell Trubisky',NULL,1),</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4272,6 +4548,112 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39725DE-07BC-4AA5-8629-15CC6A71CDD6}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" t="str" cm="1">
+        <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.Conferences(ConferenceID,Season,Name,GridColumn,GridRowStart,GridRowEnd,IsActive) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2">
+        <v>2022</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;",'"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <v>('C1',2022,'AFC',1,2,6,1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="str">
+        <f>"('"&amp;A3&amp;"',"&amp;B3&amp;",'"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <v>('C2',2022,'NFC',1,6,10,1)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -4359,7 +4741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -4617,7 +4999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4664,7 +5046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF7E11E-B54A-4612-A949-04C2EF515915}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -4723,7 +5105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1DEFA3-6198-4C61-94C1-9C389651B37A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4759,44 +5141,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Creating user registration and login
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B92A6C-15C1-49B2-921C-A0D223468490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A201CBEB-33E5-4006-8293-22AA4495F482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
     <sheet name="Teams" sheetId="1" r:id="rId2"/>
     <sheet name="Players" sheetId="3" r:id="rId3"/>
     <sheet name="Conferences" sheetId="14" r:id="rId4"/>
-    <sheet name="Users" sheetId="2" r:id="rId5"/>
-    <sheet name="PredictionPeriods" sheetId="4" r:id="rId6"/>
-    <sheet name="PeriodPredictions" sheetId="5" r:id="rId7"/>
-    <sheet name="WeekPredictions" sheetId="6" r:id="rId8"/>
-    <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId9"/>
-    <sheet name="PrivateLeagues" sheetId="8" r:id="rId10"/>
-    <sheet name="ScoringSettings" sheetId="10" r:id="rId11"/>
-    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId12"/>
-    <sheet name="UserScores" sheetId="12" r:id="rId13"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId14"/>
+    <sheet name="Roles" sheetId="15" r:id="rId5"/>
+    <sheet name="Users" sheetId="2" r:id="rId6"/>
+    <sheet name="PredictionPeriods" sheetId="4" r:id="rId7"/>
+    <sheet name="PeriodPredictions" sheetId="5" r:id="rId8"/>
+    <sheet name="WeekPredictions" sheetId="6" r:id="rId9"/>
+    <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId10"/>
+    <sheet name="PrivateLeagues" sheetId="8" r:id="rId11"/>
+    <sheet name="ScoringSettings" sheetId="10" r:id="rId12"/>
+    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
+    <sheet name="UserScores" sheetId="12" r:id="rId14"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$D$87</definedName>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="383">
   <si>
     <t>TeamID</t>
   </si>
@@ -615,9 +616,6 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>IsAuthenticated</t>
-  </si>
-  <si>
     <t>IsAdmin</t>
   </si>
   <si>
@@ -1210,6 +1208,21 @@
   </si>
   <si>
     <t>C2</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>max size 20</t>
+  </si>
+  <si>
+    <t>Roles</t>
   </si>
 </sst>
 </file>
@@ -1564,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD2AB4C-1FDF-40BE-911A-52427E1B6DC0}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1641,10 +1654,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>378</v>
+      </c>
+      <c r="B10" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -1653,6 +1674,44 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1DEFA3-6198-4C61-94C1-9C389651B37A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1692,7 +1751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1778,7 +1837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6954B5E2-894C-437E-8E51-B1D29E513C99}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1833,7 +1892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1873,7 +1932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1926,10 +1985,10 @@
         <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="K1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:I1)&amp;") VALUES"</f>
@@ -3009,7 +3068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
@@ -3025,7 +3084,7 @@
         <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>115</v>
@@ -3043,7 +3102,7 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
@@ -3061,7 +3120,7 @@
         <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3076,7 +3135,7 @@
         <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
@@ -3095,10 +3154,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -3113,10 +3172,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3128,10 +3187,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3143,10 +3202,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3158,10 +3217,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3173,10 +3232,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3191,7 +3250,7 @@
         <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3203,10 +3262,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -3221,10 +3280,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3236,10 +3295,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3251,10 +3310,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3266,10 +3325,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3281,10 +3340,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3296,10 +3355,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
@@ -3314,10 +3373,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
         <v>94</v>
@@ -3332,10 +3391,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3347,10 +3406,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
         <v>81</v>
@@ -3365,10 +3424,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -3383,10 +3442,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3398,10 +3457,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3413,10 +3472,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3428,10 +3487,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3443,10 +3502,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3458,10 +3517,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3473,10 +3532,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3488,10 +3547,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3503,10 +3562,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3518,10 +3577,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3533,10 +3592,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3548,10 +3607,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3563,10 +3622,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" t="s">
         <v>95</v>
@@ -3581,10 +3640,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C36" t="s">
         <v>99</v>
@@ -3599,10 +3658,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C37" t="s">
         <v>90</v>
@@ -3617,10 +3676,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3632,10 +3691,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C39" t="s">
         <v>103</v>
@@ -3650,10 +3709,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C40" t="s">
         <v>74</v>
@@ -3668,10 +3727,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3683,10 +3742,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3698,10 +3757,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3713,10 +3772,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B44" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C44" t="s">
         <v>77</v>
@@ -3731,10 +3790,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3746,10 +3805,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3761,10 +3820,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C47" t="s">
         <v>89</v>
@@ -3779,10 +3838,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -3797,10 +3856,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B49" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3812,10 +3871,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C50" t="s">
         <v>92</v>
@@ -3830,10 +3889,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3845,10 +3904,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3860,10 +3919,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B53" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C53" t="s">
         <v>101</v>
@@ -3878,10 +3937,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C54" t="s">
         <v>72</v>
@@ -3896,10 +3955,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3911,10 +3970,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C56" t="s">
         <v>79</v>
@@ -3929,10 +3988,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3944,10 +4003,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3959,10 +4018,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -3977,10 +4036,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
@@ -3995,10 +4054,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -4010,10 +4069,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B62" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -4025,10 +4084,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -4040,10 +4099,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -4055,10 +4114,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -4070,10 +4129,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -4085,10 +4144,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
@@ -4103,10 +4162,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B68" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -4118,10 +4177,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B69" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C69" t="s">
         <v>104</v>
@@ -4136,10 +4195,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B70" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C70" t="s">
         <v>84</v>
@@ -4154,10 +4213,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C71" t="s">
         <v>98</v>
@@ -4172,10 +4231,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -4187,10 +4246,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -4202,10 +4261,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4217,10 +4276,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
@@ -4235,10 +4294,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -4250,10 +4309,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B77" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C77" t="s">
         <v>85</v>
@@ -4268,10 +4327,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4283,10 +4342,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B79" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C79" t="s">
         <v>100</v>
@@ -4301,10 +4360,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4316,10 +4375,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C81" t="s">
         <v>83</v>
@@ -4334,10 +4393,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B82" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4349,10 +4408,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B83" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4364,10 +4423,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C84" t="s">
         <v>78</v>
@@ -4382,10 +4441,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4397,10 +4456,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -4412,10 +4471,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B87" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C87" t="s">
         <v>80</v>
@@ -4430,10 +4489,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B88" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4445,10 +4504,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B89" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4460,10 +4519,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B90" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4475,10 +4534,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B91" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4490,10 +4549,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B92" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4505,10 +4564,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B93" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4520,10 +4579,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B94" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4568,22 +4627,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>134</v>
@@ -4595,7 +4654,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -4622,7 +4681,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -4654,10 +4713,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142D061-4F37-4CE5-9EF1-93D58F744102}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4666,13 +4751,12 @@
     <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>105</v>
       </c>
@@ -4689,19 +4773,16 @@
         <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -4717,21 +4798,20 @@
       <c r="E2" t="s">
         <v>112</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="H2" s="3">
         <v>44591.015905787041</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I3" s="3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>381</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4741,7 +4821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -4765,7 +4845,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>122</v>
@@ -4925,7 +5005,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7">
         <v>2023</v>
@@ -4939,7 +5019,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B8">
         <v>2023</v>
@@ -4953,7 +5033,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B9">
         <v>2023</v>
@@ -4967,7 +5047,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B10">
         <v>2023</v>
@@ -4981,7 +5061,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B11">
         <v>2023</v>
@@ -4999,7 +5079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -5046,7 +5126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF7E11E-B54A-4612-A949-04C2EF515915}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -5103,42 +5183,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1DEFA3-6198-4C61-94C1-9C389651B37A}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Preparing for user registration
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A201CBEB-33E5-4006-8293-22AA4495F482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB76558-51C3-40E4-A6FB-02138A3DD432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,12 +397,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>EmailAddress</t>
-  </si>
-  <si>
-    <t>HashedPassword</t>
-  </si>
-  <si>
     <t>UserCreated</t>
   </si>
   <si>
@@ -1223,6 +1217,12 @@
   </si>
   <si>
     <t>Roles</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1590,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1601,60 +1601,60 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -1689,7 +1689,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>105</v>
@@ -1697,13 +1697,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1726,13 +1726,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1740,10 +1740,10 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1765,33 +1765,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1811,10 +1811,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1849,7 +1849,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>105</v>
@@ -1860,7 +1860,7 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1868,7 +1868,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1876,7 +1876,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1884,7 +1884,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1907,21 +1907,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>0.875</v>
@@ -1982,13 +1982,13 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:I1)&amp;") VALUES"</f>
@@ -2204,7 +2204,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -2300,7 +2300,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -2765,7 +2765,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -3081,16 +3081,16 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F1" t="str" cm="1">
         <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
@@ -3099,10 +3099,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
@@ -3117,10 +3117,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -3172,10 +3172,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3187,10 +3187,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3202,10 +3202,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3217,10 +3217,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3262,10 +3262,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3310,10 +3310,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3325,10 +3325,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3355,10 +3355,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
@@ -3373,10 +3373,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
         <v>94</v>
@@ -3391,10 +3391,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3406,10 +3406,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
         <v>81</v>
@@ -3424,10 +3424,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -3442,10 +3442,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3457,10 +3457,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3487,10 +3487,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3517,10 +3517,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3532,10 +3532,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3547,10 +3547,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3562,10 +3562,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3577,10 +3577,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3592,10 +3592,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3607,10 +3607,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3622,10 +3622,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C35" t="s">
         <v>95</v>
@@ -3640,10 +3640,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B36" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
         <v>99</v>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C37" t="s">
         <v>90</v>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3691,10 +3691,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C39" t="s">
         <v>103</v>
@@ -3709,10 +3709,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B40" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C40" t="s">
         <v>74</v>
@@ -3727,10 +3727,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3742,10 +3742,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3757,10 +3757,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3772,10 +3772,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C44" t="s">
         <v>77</v>
@@ -3790,10 +3790,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B45" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3805,10 +3805,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3820,10 +3820,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B47" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C47" t="s">
         <v>89</v>
@@ -3838,10 +3838,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -3856,10 +3856,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B49" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3871,10 +3871,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C50" t="s">
         <v>92</v>
@@ -3889,10 +3889,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B51" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3904,10 +3904,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B52" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3919,10 +3919,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B53" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C53" t="s">
         <v>101</v>
@@ -3937,10 +3937,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B54" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C54" t="s">
         <v>72</v>
@@ -3955,10 +3955,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B55" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C56" t="s">
         <v>79</v>
@@ -3988,10 +3988,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B57" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -4003,10 +4003,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B58" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -4018,10 +4018,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B59" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -4036,10 +4036,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B60" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
@@ -4054,10 +4054,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -4069,10 +4069,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B62" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -4084,10 +4084,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -4099,10 +4099,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B64" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -4114,10 +4114,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -4129,10 +4129,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B66" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -4144,10 +4144,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B67" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
@@ -4162,10 +4162,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B68" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -4177,10 +4177,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B69" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C69" t="s">
         <v>104</v>
@@ -4195,10 +4195,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C70" t="s">
         <v>84</v>
@@ -4213,10 +4213,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C71" t="s">
         <v>98</v>
@@ -4231,10 +4231,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B72" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -4246,10 +4246,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B73" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -4261,10 +4261,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4276,10 +4276,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
@@ -4294,10 +4294,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B76" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -4309,10 +4309,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B77" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C77" t="s">
         <v>85</v>
@@ -4327,10 +4327,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4342,10 +4342,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B79" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C79" t="s">
         <v>100</v>
@@ -4360,10 +4360,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4375,10 +4375,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B81" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C81" t="s">
         <v>83</v>
@@ -4393,10 +4393,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B82" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4408,10 +4408,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B83" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4423,10 +4423,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B84" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C84" t="s">
         <v>78</v>
@@ -4441,10 +4441,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4456,10 +4456,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -4471,10 +4471,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C87" t="s">
         <v>80</v>
@@ -4489,10 +4489,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B88" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4504,10 +4504,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B89" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4519,10 +4519,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B90" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4534,10 +4534,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B91" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4549,10 +4549,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B92" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4564,10 +4564,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B93" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4579,10 +4579,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B94" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4627,25 +4627,25 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I1" t="str" cm="1">
         <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -4724,10 +4724,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4741,7 +4741,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4764,39 +4764,39 @@
         <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" t="s">
-        <v>112</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4839,42 +4839,42 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" s="3">
         <v>44449.013888888891</v>
@@ -4893,16 +4893,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" s="3">
         <v>44569.895833333336</v>
@@ -4921,16 +4921,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E4" s="3">
         <v>44603.979166666664</v>
@@ -4949,16 +4949,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" s="3">
         <v>44636.833333333336</v>
@@ -4977,16 +4977,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6">
         <v>2022</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E6" s="3">
         <v>44680</v>
@@ -5005,72 +5005,72 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B7">
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B8">
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B9">
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B10">
         <v>2023</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B11">
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -5095,7 +5095,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>105</v>
@@ -5104,21 +5104,21 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -5145,10 +5145,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>105</v>
@@ -5157,27 +5157,27 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Able to create users using API
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB76558-51C3-40E4-A6FB-02138A3DD432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04023200-0995-4488-A1DF-AFED453FBB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="392">
   <si>
     <t>TeamID</t>
   </si>
@@ -1223,6 +1223,33 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>ROLE_USER</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>ROLE_MODERATOR</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>ROLE_ADMIN</t>
+  </si>
+  <si>
+    <t>INSERT INTO roles(roleid,name) VALUES('R1','ROLE_USER');</t>
+  </si>
+  <si>
+    <t>INSERT INTO roles(roleid,name) VALUES('R2','ROLE_MODERATOR');</t>
+  </si>
+  <si>
+    <t>INSERT INTO roles(roleid,name) VALUES('R3','ROLE_ADMIN');</t>
   </si>
 </sst>
 </file>
@@ -1289,13 +1316,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4714,20 +4744,57 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142D061-4F37-4CE5-9EF1-93D58F744102}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>378</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -4740,7 +4807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Automating the prediction period table visualisation
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04023200-0995-4488-A1DF-AFED453FBB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF8681F-462A-401C-A877-2B31C563DA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="Roles" sheetId="15" r:id="rId5"/>
     <sheet name="Users" sheetId="2" r:id="rId6"/>
     <sheet name="PredictionPeriods" sheetId="4" r:id="rId7"/>
-    <sheet name="PeriodPredictions" sheetId="5" r:id="rId8"/>
-    <sheet name="WeekPredictions" sheetId="6" r:id="rId9"/>
-    <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId10"/>
-    <sheet name="PrivateLeagues" sheetId="8" r:id="rId11"/>
-    <sheet name="ScoringSettings" sheetId="10" r:id="rId12"/>
-    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
-    <sheet name="UserScores" sheetId="12" r:id="rId14"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId15"/>
+    <sheet name="Events" sheetId="16" r:id="rId8"/>
+    <sheet name="PeriodPredictions" sheetId="5" r:id="rId9"/>
+    <sheet name="WeekPredictions" sheetId="6" r:id="rId10"/>
+    <sheet name="UserPeriodPredictions" sheetId="7" r:id="rId11"/>
+    <sheet name="PrivateLeagues" sheetId="8" r:id="rId12"/>
+    <sheet name="ScoringSettings" sheetId="10" r:id="rId13"/>
+    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId14"/>
+    <sheet name="UserScores" sheetId="12" r:id="rId15"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$D$87</definedName>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="404">
   <si>
     <t>TeamID</t>
   </si>
@@ -430,30 +431,9 @@
     <t>PredictionPeriodID</t>
   </si>
   <si>
-    <t>ToDateTime</t>
-  </si>
-  <si>
-    <t>FromDateTime</t>
-  </si>
-  <si>
-    <t>DeadlineEvent</t>
-  </si>
-  <si>
-    <t>First KO of 2021 Week 18</t>
-  </si>
-  <si>
     <t>KO of Super Bowl LVI</t>
   </si>
   <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Free Agency begins</t>
-  </si>
-  <si>
-    <t>NFL Draft</t>
-  </si>
-  <si>
     <t>PP1</t>
   </si>
   <si>
@@ -469,9 +449,6 @@
     <t>PP5</t>
   </si>
   <si>
-    <t>Weeks</t>
-  </si>
-  <si>
     <t>IsActive</t>
   </si>
   <si>
@@ -559,18 +536,9 @@
     <t>SP4</t>
   </si>
   <si>
-    <t>First KO of 2022 Week 18</t>
-  </si>
-  <si>
     <t>KO of Super Bowl LVII</t>
   </si>
   <si>
-    <t>First KO of 2023 Week 1</t>
-  </si>
-  <si>
-    <t>First KO of 2022 Week 1 (date tbc)</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
@@ -1174,12 +1142,6 @@
     <t>PP8</t>
   </si>
   <si>
-    <t>PP9</t>
-  </si>
-  <si>
-    <t>PP10</t>
-  </si>
-  <si>
     <t>GridColumn</t>
   </si>
   <si>
@@ -1250,6 +1212,81 @@
   </si>
   <si>
     <t>INSERT INTO roles(roleid,name) VALUES('R3','ROLE_ADMIN');</t>
+  </si>
+  <si>
+    <t>EventID</t>
+  </si>
+  <si>
+    <t>EventName</t>
+  </si>
+  <si>
+    <t>DateConfirmed</t>
+  </si>
+  <si>
+    <t>KO of 2022 Regular Season opener</t>
+  </si>
+  <si>
+    <t>KO of 2021 Regular Season opener</t>
+  </si>
+  <si>
+    <t>EventDateTimeUTC</t>
+  </si>
+  <si>
+    <t>Start of 2022 League Year and Free Agency</t>
+  </si>
+  <si>
+    <t>Start of 2022 NFL Draft</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>Start of 2023 League Year and Free Agency</t>
+  </si>
+  <si>
+    <t>Start of 2023 NFL Draft</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>FromEventID</t>
+  </si>
+  <si>
+    <t>ToEventID</t>
+  </si>
+  <si>
+    <t>KO of 1st game in final round of 2022 Regular Season games</t>
+  </si>
+  <si>
+    <t>KO of 1st game in final round of 2021 Regular Season games</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>HowItWorks</t>
   </si>
 </sst>
 </file>
@@ -1620,10 +1657,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1631,60 +1668,60 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1692,10 +1729,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="B10" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -1704,6 +1741,65 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF7E11E-B54A-4612-A949-04C2EF515915}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1DEFA3-6198-4C61-94C1-9C389651B37A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1727,13 +1823,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +1837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1756,13 +1852,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1773,7 +1869,7 @@
         <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +1877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1795,33 +1891,33 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
         <v>156</v>
-      </c>
-      <c r="B2" t="s">
-        <v>167</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -1841,10 +1937,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>0.24419428096993967</v>
@@ -1867,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6954B5E2-894C-437E-8E51-B1D29E513C99}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1879,7 +1975,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>105</v>
@@ -1898,7 +1994,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1906,7 +2002,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1914,7 +2010,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1922,7 +2018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1943,12 +2039,12 @@
         <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>111</v>
@@ -1962,7 +2058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1978,7 +2074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K33"/>
     </sheetView>
   </sheetViews>
@@ -2012,13 +2108,13 @@
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="K1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:I1)&amp;") VALUES"</f>
@@ -2234,7 +2330,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -2330,7 +2426,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -2795,7 +2891,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -3098,8 +3194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3114,13 +3210,13 @@
         <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F1" t="str" cm="1">
         <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
@@ -3132,7 +3228,7 @@
         <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
@@ -3150,7 +3246,7 @@
         <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3165,7 +3261,7 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
@@ -3184,10 +3280,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -3202,10 +3298,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B6" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3217,10 +3313,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3232,10 +3328,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -3247,10 +3343,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3262,10 +3358,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3277,10 +3373,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3292,10 +3388,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
         <v>82</v>
@@ -3310,10 +3406,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3325,10 +3421,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B14" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3340,10 +3436,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3355,10 +3451,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B16" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3370,10 +3466,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B17" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3385,10 +3481,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B18" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
@@ -3403,10 +3499,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B19" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C19" t="s">
         <v>94</v>
@@ -3421,10 +3517,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3436,10 +3532,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B21" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
         <v>81</v>
@@ -3454,10 +3550,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -3472,10 +3568,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3487,10 +3583,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3502,10 +3598,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3517,10 +3613,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3532,10 +3628,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3547,10 +3643,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="B28" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3562,10 +3658,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B29" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3577,10 +3673,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3592,10 +3688,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="B31" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3607,10 +3703,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B32" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3622,10 +3718,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3637,10 +3733,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B34" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3652,10 +3748,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B35" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C35" t="s">
         <v>95</v>
@@ -3670,10 +3766,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C36" t="s">
         <v>99</v>
@@ -3688,10 +3784,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
         <v>90</v>
@@ -3706,10 +3802,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3721,10 +3817,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B39" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
         <v>103</v>
@@ -3739,10 +3835,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="B40" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C40" t="s">
         <v>74</v>
@@ -3757,10 +3853,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3772,10 +3868,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="B42" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3787,10 +3883,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="B43" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3802,10 +3898,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="B44" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C44" t="s">
         <v>77</v>
@@ -3820,10 +3916,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B45" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3835,10 +3931,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B46" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3850,10 +3946,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B47" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C47" t="s">
         <v>89</v>
@@ -3868,10 +3964,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B48" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -3886,10 +3982,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3901,10 +3997,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B50" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C50" t="s">
         <v>92</v>
@@ -3919,10 +4015,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3934,10 +4030,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="B52" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3949,10 +4045,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="B53" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C53" t="s">
         <v>101</v>
@@ -3967,10 +4063,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B54" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C54" t="s">
         <v>72</v>
@@ -3985,10 +4081,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="B55" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -4000,10 +4096,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
         <v>79</v>
@@ -4018,10 +4114,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="B57" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -4033,10 +4129,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="B58" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -4048,10 +4144,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C59" t="s">
         <v>97</v>
@@ -4066,10 +4162,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="B60" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
@@ -4084,10 +4180,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="B61" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -4099,10 +4195,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B62" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -4114,10 +4210,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -4129,10 +4225,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B64" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -4144,10 +4240,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B65" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -4159,10 +4255,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="B66" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -4174,10 +4270,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="B67" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
@@ -4192,10 +4288,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B68" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -4207,10 +4303,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B69" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C69" t="s">
         <v>104</v>
@@ -4225,10 +4321,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B70" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C70" t="s">
         <v>84</v>
@@ -4243,10 +4339,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B71" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C71" t="s">
         <v>98</v>
@@ -4261,10 +4357,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -4276,10 +4372,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="B73" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -4291,10 +4387,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B74" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4306,10 +4402,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="B75" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
@@ -4324,10 +4420,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="B76" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -4339,10 +4435,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C77" t="s">
         <v>85</v>
@@ -4357,10 +4453,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="B78" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4372,10 +4468,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="B79" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C79" t="s">
         <v>100</v>
@@ -4390,10 +4486,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B80" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4405,10 +4501,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B81" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C81" t="s">
         <v>83</v>
@@ -4423,10 +4519,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4438,10 +4534,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="B83" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4453,10 +4549,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C84" t="s">
         <v>78</v>
@@ -4471,10 +4567,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4486,10 +4582,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="B86" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -4501,10 +4597,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="B87" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C87" t="s">
         <v>80</v>
@@ -4519,10 +4615,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B88" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4534,10 +4630,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="B89" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4549,10 +4645,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="B90" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4564,10 +4660,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="B91" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4579,10 +4675,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="B92" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4594,10 +4690,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="B93" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4609,10 +4705,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="B94" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4657,25 +4753,25 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I1" t="str" cm="1">
         <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
@@ -4684,7 +4780,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="B2">
         <v>2022</v>
@@ -4711,7 +4807,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -4746,7 +4842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142D061-4F37-4CE5-9EF1-93D58F744102}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -4758,43 +4854,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="D3" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="D4" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -4831,19 +4927,19 @@
         <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>107</v>
@@ -4860,7 +4956,7 @@
         <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
         <v>110</v>
@@ -4877,7 +4973,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -4890,21 +4986,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>117</v>
       </c>
@@ -4912,232 +5010,239 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>397</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" t="str" cm="1">
+        <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.PredictionPeriods(PredictionPeriodID,Season,SeasonPeriodID,FromEventID,ToEventID,HowItWorks,IsActive) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>119</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>126</v>
       </c>
       <c r="B2">
         <v>2022</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="3">
-        <v>44449.013888888891</v>
-      </c>
-      <c r="F2" s="3">
-        <v>44569.895833333336</v>
+        <v>387</v>
+      </c>
+      <c r="E2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2">
-        <f>F2-E2</f>
-        <v>120.88194444444525</v>
-      </c>
-      <c r="H2">
-        <f>G2/7</f>
-        <v>17.268849206349323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"',"&amp;F2&amp;","&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <v>('PP1',2022,'SP1','E1','E2',1,1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="3">
-        <v>44569.895833333336</v>
-      </c>
-      <c r="F3" s="3">
-        <v>44603.979166666664</v>
+        <v>388</v>
+      </c>
+      <c r="E3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
       </c>
       <c r="G3">
-        <f>F3-E3</f>
-        <v>34.083333333328483</v>
-      </c>
-      <c r="H3">
-        <f>G3/7</f>
-        <v>4.8690476190469258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I9" si="0">"('"&amp;A3&amp;"',"&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"',"&amp;F3&amp;","&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <v>('PP2',2022,'SP2','E2','E3',1,1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>2022</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="3">
-        <v>44603.979166666664</v>
-      </c>
-      <c r="F4" s="3">
-        <v>44636.833333333336</v>
+        <v>389</v>
+      </c>
+      <c r="E4" t="s">
+        <v>390</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4">
-        <f>F4-E4</f>
-        <v>32.854166666671517</v>
-      </c>
-      <c r="H4">
-        <f>G4/7</f>
-        <v>4.6934523809530742</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>('PP3',2022,'SP3','E3','E4',1,1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="3">
-        <v>44636.833333333336</v>
-      </c>
-      <c r="F5" s="3">
-        <v>44680</v>
+        <v>390</v>
+      </c>
+      <c r="E5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
       </c>
       <c r="G5">
-        <f>F5-E5</f>
-        <v>43.166666666664241</v>
-      </c>
-      <c r="H5">
-        <f>G5/7</f>
-        <v>6.1666666666663206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>('PP4',2022,'SP4','E4','E5',1,1),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B6">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="3">
-        <v>44680</v>
-      </c>
-      <c r="F6" s="3">
-        <v>44812.013888888891</v>
+        <v>394</v>
+      </c>
+      <c r="E6" t="s">
+        <v>395</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6">
-        <f>F6-E6</f>
-        <v>132.01388888889051</v>
-      </c>
-      <c r="H6">
-        <f>G6/7</f>
-        <v>18.859126984127215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>('PP5',2023,'SP1','E6','E7',0,1),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="B7">
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+      <c r="E7" t="s">
+        <v>396</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>('PP6',2023,'SP2','E7','E8',0,1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B8">
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+      <c r="E8" t="s">
+        <v>401</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>('PP7',2023,'SP3','E8','E9',0,1),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="B9">
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>366</v>
-      </c>
-      <c r="B10">
-        <v>2023</v>
-      </c>
-      <c r="C10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>367</v>
-      </c>
-      <c r="B11">
-        <v>2023</v>
-      </c>
-      <c r="C11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" t="s">
-        <v>163</v>
+        <v>401</v>
+      </c>
+      <c r="E9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>('PP8',2023,'SP4','E9','E10',0,1)</v>
       </c>
     </row>
   </sheetData>
@@ -5147,6 +5252,239 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F502399-C795-4D5E-88DC-92C8B5181153}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1" t="str" cm="1">
+        <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.Events(EventID,EventName,EventDateTimeUTC,DateConfirmed) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44449.013888888891</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"('"&amp;A2&amp;"','"&amp;B2&amp;"',"&amp;IF(LEN(C2)&gt;0,"'"&amp;TEXT(C2,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <v>('E1','KO of 2021 Regular Season opener','2021-09-10 00:20',1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44569.895833333336</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F11" si="0">"('"&amp;A3&amp;"','"&amp;B3&amp;"',"&amp;IF(LEN(C3)&gt;0,"'"&amp;TEXT(C3,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <v>('E2','KO of 1st game in final round of 2021 Regular Season games','2022-01-08 21:30',1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44605.979166666664</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>('E3','KO of Super Bowl LVI','2022-02-13 23:30',1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44636.833333333336</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>('E4','Start of 2022 League Year and Free Agency','2022-03-16 20:00',1),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B6" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44680</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>('E5','Start of 2022 NFL Draft','2022-04-29 00:00',0),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44813.013888888891</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>('E6','KO of 2022 Regular Season opener','2022-09-09 00:20',0),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44570.895833333336</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>('E7','KO of 1st game in final round of 2022 Regular Season games','2022-01-09 21:30',0),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>396</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44604.979166666664</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>('E8','KO of Super Bowl LVII','2022-02-12 23:30',0),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>401</v>
+      </c>
+      <c r="B10" t="s">
+        <v>391</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45000.833333333336</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>('E9','Start of 2023 League Year and Free Agency','2023-03-15 20:00',0),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>402</v>
+      </c>
+      <c r="B11" t="s">
+        <v>392</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45044</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>('E10','Start of 2023 NFL Draft','2023-04-28 00:00',0)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="str">
+        <f>YEAR(C2)&amp;"-"&amp;MONTH(C2)&amp;"-"&amp;DAY(C2)</f>
+        <v>2021-9-10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="str">
+        <f>TEXT(C2,"YYYY-MM-DD HH:MM")</f>
+        <v>2021-09-10 00:20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -5176,7 +5514,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>111</v>
@@ -5185,66 +5523,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF7E11E-B54A-4612-A949-04C2EF515915}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All joins created, basic testing needed before merge
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BEB3B6-DBC4-44DD-B7F4-10BB2CA55438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F90AC0F-166F-4880-9919-C40DC4C7077D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -23,10 +23,11 @@
     <sheet name="Events" sheetId="16" r:id="rId8"/>
     <sheet name="PeriodPredictions" sheetId="5" r:id="rId9"/>
     <sheet name="PrivateLeagues" sheetId="8" r:id="rId10"/>
-    <sheet name="ScoringSettings" sheetId="10" r:id="rId11"/>
-    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId12"/>
-    <sheet name="UserScores" sheetId="12" r:id="rId13"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId14"/>
+    <sheet name="ScoringSettingsValues" sheetId="10" r:id="rId11"/>
+    <sheet name="ScoringSettings" sheetId="17" r:id="rId12"/>
+    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
+    <sheet name="UserScores" sheetId="12" r:id="rId14"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$D$94</definedName>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="254">
   <si>
     <t>TeamID</t>
   </si>
@@ -393,21 +394,6 @@
     <t>SeasonPeriod</t>
   </si>
   <si>
-    <t>SP1</t>
-  </si>
-  <si>
-    <t>SP5</t>
-  </si>
-  <si>
-    <t>SP2</t>
-  </si>
-  <si>
-    <t>SP3</t>
-  </si>
-  <si>
-    <t>SP4</t>
-  </si>
-  <si>
     <t>KO of Super Bowl LVII</t>
   </si>
   <si>
@@ -841,6 +827,15 @@
   </si>
   <si>
     <t>DefaultPlayerID</t>
+  </si>
+  <si>
+    <t>ScoringPeriodID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ScoringSettingID</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1262,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
         <v>105</v>
@@ -1275,7 +1270,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1283,10 +1278,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1331,93 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC4630A-EA58-44F8-89AC-CF1055B6051C}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1346,73 +1427,28 @@
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>110</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2">
-        <v>0.2</v>
-      </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-      <c r="E2">
-        <v>0.2</v>
-      </c>
-      <c r="F2">
-        <v>0.2</v>
-      </c>
-      <c r="G2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3">
-        <v>0.24419428096993967</v>
-      </c>
-      <c r="D3">
-        <v>0.21977485287294571</v>
-      </c>
-      <c r="E3">
-        <v>0.19779736758565114</v>
-      </c>
-      <c r="F3">
-        <v>0.17801763082708602</v>
-      </c>
-      <c r="G3">
-        <v>0.16021586774437743</v>
       </c>
     </row>
   </sheetData>
@@ -1420,7 +1456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6954B5E2-894C-437E-8E51-B1D29E513C99}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1451,7 +1487,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1459,7 +1495,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1467,7 +1503,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1496,7 +1532,7 @@
         <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1515,7 +1551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1531,7 +1567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -1569,13 +1605,13 @@
         <v>86</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:J1)&amp;") VALUES"</f>
@@ -1809,7 +1845,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -1914,7 +1950,7 @@
         <v>2022</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
         <v>55</v>
@@ -2421,7 +2457,7 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2768,7 +2804,7 @@
         <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>82</v>
@@ -2786,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C2">
         <v>19</v>
@@ -2804,7 +2840,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2819,7 +2855,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2841,7 +2877,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2859,7 +2895,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2874,7 +2910,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2889,7 +2925,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2904,7 +2940,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2919,7 +2955,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2934,7 +2970,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2949,7 +2985,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -2967,7 +3003,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2982,7 +3018,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2997,7 +3033,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3012,7 +3048,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3027,7 +3063,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3042,7 +3078,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C18">
         <v>21</v>
@@ -3060,7 +3096,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C19">
         <v>22</v>
@@ -3078,7 +3114,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3093,7 +3129,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -3111,7 +3147,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -3129,7 +3165,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3144,7 +3180,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3159,7 +3195,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3174,7 +3210,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3189,7 +3225,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3204,7 +3240,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3219,7 +3255,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3234,7 +3270,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3249,7 +3285,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3264,7 +3300,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3279,7 +3315,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3294,7 +3330,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3309,7 +3345,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C35">
         <v>23</v>
@@ -3327,7 +3363,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C36">
         <v>27</v>
@@ -3345,7 +3381,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C37">
         <v>18</v>
@@ -3363,7 +3399,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3378,7 +3414,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C39">
         <v>31</v>
@@ -3396,7 +3432,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3414,7 +3450,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3429,7 +3465,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3444,7 +3480,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3459,7 +3495,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -3477,7 +3513,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3492,7 +3528,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3507,7 +3543,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C47">
         <v>17</v>
@@ -3525,7 +3561,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C48">
         <v>16</v>
@@ -3543,7 +3579,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3558,7 +3594,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C50">
         <v>20</v>
@@ -3576,7 +3612,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3591,7 +3627,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3606,7 +3642,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C53">
         <v>29</v>
@@ -3624,7 +3660,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3642,7 +3678,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3657,7 +3693,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C56">
         <v>7</v>
@@ -3675,7 +3711,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3690,7 +3726,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3705,7 +3741,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C59">
         <v>25</v>
@@ -3723,7 +3759,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C60">
         <v>30</v>
@@ -3741,7 +3777,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -3756,7 +3792,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3771,7 +3807,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -3786,7 +3822,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3801,7 +3837,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -3816,7 +3852,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -3831,7 +3867,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C67">
         <v>14</v>
@@ -3849,7 +3885,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -3864,7 +3900,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C69">
         <v>32</v>
@@ -3882,7 +3918,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C70">
         <v>12</v>
@@ -3900,7 +3936,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C71">
         <v>26</v>
@@ -3918,7 +3954,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -3933,7 +3969,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -3948,7 +3984,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -3963,7 +3999,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C75">
         <v>24</v>
@@ -3981,7 +4017,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -3996,7 +4032,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C77">
         <v>13</v>
@@ -4014,7 +4050,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4029,7 +4065,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C79">
         <v>28</v>
@@ -4047,7 +4083,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4062,7 +4098,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C81">
         <v>11</v>
@@ -4080,7 +4116,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4095,7 +4131,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4110,7 +4146,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C84">
         <v>6</v>
@@ -4128,7 +4164,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4143,7 +4179,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -4158,7 +4194,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C87">
         <v>8</v>
@@ -4176,7 +4212,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4191,7 +4227,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4206,7 +4242,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4221,7 +4257,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4236,7 +4272,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4251,7 +4287,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4266,7 +4302,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4316,22 +4352,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>86</v>
@@ -4417,10 +4453,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4428,10 +4464,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -4439,10 +4475,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4450,10 +4486,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4490,19 +4526,19 @@
         <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>76</v>
@@ -4519,7 +4555,7 @@
         <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
         <v>79</v>
@@ -4536,7 +4572,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -4573,16 +4609,16 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>86</v>
@@ -4832,16 +4868,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F1" t="str" cm="1">
         <f t="array" aca="1" ref="F1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:D1)&amp;") VALUES"</f>
@@ -4853,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C2" s="3">
         <v>44449.013888888891</v>
@@ -4871,7 +4907,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C3" s="3">
         <v>44569.895833333336</v>
@@ -4907,7 +4943,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C5" s="3">
         <v>44636.833333333336</v>
@@ -4925,7 +4961,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C6" s="3">
         <v>44680</v>
@@ -4943,7 +4979,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C7" s="3">
         <v>44813.013888888891</v>
@@ -4961,7 +4997,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C8" s="3">
         <v>44935.895833333336</v>
@@ -4979,7 +5015,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C9" s="3">
         <v>44969.979166666664</v>
@@ -4997,7 +5033,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C10" s="3">
         <v>45000.833333333336</v>
@@ -5015,7 +5051,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C11" s="3">
         <v>45044</v>

</xml_diff>

<commit_message>
Continue work on answer entry page
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B65BC5E-4707-4AD8-ABCB-E3F79BF8D98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763CEF8E-670B-46C8-BEF7-39001C141E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="833" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="Players" sheetId="3" r:id="rId3"/>
     <sheet name="Conferences" sheetId="14" r:id="rId4"/>
     <sheet name="Roles" sheetId="15" r:id="rId5"/>
-    <sheet name="Users" sheetId="2" r:id="rId6"/>
-    <sheet name="PredictionPeriods" sheetId="4" r:id="rId7"/>
-    <sheet name="Events" sheetId="16" r:id="rId8"/>
-    <sheet name="PeriodPredictions" sheetId="5" r:id="rId9"/>
-    <sheet name="PrivateLeagues" sheetId="8" r:id="rId10"/>
-    <sheet name="ScoringSettings" sheetId="10" r:id="rId11"/>
-    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId12"/>
-    <sheet name="UserScores" sheetId="12" r:id="rId13"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId14"/>
+    <sheet name="AnswerTypes" sheetId="17" r:id="rId6"/>
+    <sheet name="Users" sheetId="2" r:id="rId7"/>
+    <sheet name="PredictionPeriods" sheetId="4" r:id="rId8"/>
+    <sheet name="Events" sheetId="16" r:id="rId9"/>
+    <sheet name="PeriodPredictions" sheetId="5" r:id="rId10"/>
+    <sheet name="PrivateLeagues" sheetId="8" r:id="rId11"/>
+    <sheet name="ScoringSettings" sheetId="10" r:id="rId12"/>
+    <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
+    <sheet name="UserScores" sheetId="12" r:id="rId14"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$D$87</definedName>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="265">
   <si>
     <t>TeamID</t>
   </si>
@@ -838,6 +839,36 @@
   </si>
   <si>
     <t>INSERT INTO roles(roleid,name) VALUES(3,'ROLE_ADMIN');</t>
+  </si>
+  <si>
+    <t>AnswerTypeID</t>
+  </si>
+  <si>
+    <t>AnswerType</t>
+  </si>
+  <si>
+    <t>AnswerTypeTidy</t>
+  </si>
+  <si>
+    <t>ANSWERTYPE_PREVIOUS_SEASON_STARTER</t>
+  </si>
+  <si>
+    <t>ANSWERTYPE_DRAFTED</t>
+  </si>
+  <si>
+    <t>ANSWERTYPE_VETERAN</t>
+  </si>
+  <si>
+    <t>Newly Drafted QB</t>
+  </si>
+  <si>
+    <t>Veteran QB</t>
+  </si>
+  <si>
+    <t>Last Season''s Starter</t>
+  </si>
+  <si>
+    <t>INSERT INTO the_qb_carousel.answertypes (answertypeid,answertype,answertypetidy) VALUES</t>
   </si>
 </sst>
 </file>
@@ -1292,6 +1323,53 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2A964-6D6F-40DF-AB3E-3D03D24B0F24}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1331,7 +1409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1417,7 +1495,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6954B5E2-894C-437E-8E51-B1D29E513C99}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1472,7 +1550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1512,7 +1590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4354,6 +4432,86 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C582A1-DAB7-4D0D-8EF2-2F24E7E5CA97}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"')"&amp;IF(LEN(A3)&gt;0,",",";")</f>
+        <v>(1,'ANSWERTYPE_PREVIOUS_SEASON_STARTER','Last Season''s Starter'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E4" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"')"&amp;IF(LEN(A4)&gt;0,",",";")</f>
+        <v>(2,'ANSWERTYPE_DRAFTED','Newly Drafted QB'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'ANSWERTYPE_VETERAN','Veteran QB');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A1A9A1-6B63-4A68-8D84-8695BA25B5B3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -4438,11 +4596,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I1:I9"/>
     </sheetView>
   </sheetViews>
@@ -4705,7 +4863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F502399-C795-4D5E-88DC-92C8B5181153}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -4936,51 +5094,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E69C3-B83B-40BE-8CF0-32DEF1FF971E}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Answer table formatted, now onto modal entry
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763CEF8E-670B-46C8-BEF7-39001C141E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B98381D-649B-4CF4-B7C1-CA5E7FB91B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="277">
   <si>
     <t>TeamID</t>
   </si>
@@ -869,6 +869,42 @@
   </si>
   <si>
     <t>INSERT INTO the_qb_carousel.answertypes (answertypeid,answertype,answertypetidy) VALUES</t>
+  </si>
+  <si>
+    <t>Bryce Young</t>
+  </si>
+  <si>
+    <t>update PJ</t>
+  </si>
+  <si>
+    <t>CJ Stroud</t>
+  </si>
+  <si>
+    <t>Will Levis</t>
+  </si>
+  <si>
+    <t>Hendon Hooker</t>
+  </si>
+  <si>
+    <t>Anthony Richardson</t>
+  </si>
+  <si>
+    <t>Tyler Van Dyke</t>
+  </si>
+  <si>
+    <t>Tanner McKee</t>
+  </si>
+  <si>
+    <t>KJ Jefferson</t>
+  </si>
+  <si>
+    <t>Jaren Hall</t>
+  </si>
+  <si>
+    <t>Jayden Daniels</t>
+  </si>
+  <si>
+    <t>Malik Cunningham</t>
   </si>
 </sst>
 </file>
@@ -2724,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F94"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4248,6 +4284,66 @@
       <c r="F94" t="str">
         <f t="shared" si="1"/>
         <v>(93,'Sam Howell',NULL,1)</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -4435,7 +4531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C582A1-DAB7-4D0D-8EF2-2F24E7E5CA97}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Prediction history dropdown working
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B98381D-649B-4CF4-B7C1-CA5E7FB91B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AADBB49-0443-42F0-8A65-91C6BE437A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>

</xml_diff>

<commit_message>
Cleaned up how it works
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9725882D-E02F-4F61-858D-E0407A5BCC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771B0897-7FA7-4478-AE68-662D1C28DD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -3927,7 +3927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB509DC1-998D-4BFD-AC70-46B5E715D944}">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
@@ -3966,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"',"&amp;C2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <f t="shared" ref="E2:E33" si="0">"("&amp;A2&amp;",'"&amp;B2&amp;"',"&amp;C2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
         <v>(1,'Aaron Rodgers',1),</v>
       </c>
       <c r="I2" s="9"/>
@@ -3985,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="str">
-        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"',"&amp;C3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(2,'Andy Dalton',1),</v>
       </c>
       <c r="I3" s="9"/>
@@ -4004,7 +4004,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <f>"("&amp;A4&amp;",'"&amp;B4&amp;"',"&amp;C4&amp;")"&amp;IF(LEN(A5)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(3,'Baker Mayfield',1),</v>
       </c>
       <c r="I4" s="9"/>
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="str">
-        <f>"("&amp;A5&amp;",'"&amp;B5&amp;"',"&amp;C5&amp;")"&amp;IF(LEN(A6)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(4,'Ben Roethlisberger',0),</v>
       </c>
       <c r="I5" s="9"/>
@@ -4041,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <f>"("&amp;A6&amp;",'"&amp;B6&amp;"',"&amp;C6&amp;")"&amp;IF(LEN(A7)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(5,'Blaine Gabbert',1),</v>
       </c>
       <c r="I6" s="9"/>
@@ -4059,7 +4059,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <f>"("&amp;A7&amp;",'"&amp;B7&amp;"',"&amp;C7&amp;")"&amp;IF(LEN(A8)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(6,'Brandon Allen',1),</v>
       </c>
       <c r="I7" s="9"/>
@@ -4078,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <f>"("&amp;A8&amp;",'"&amp;B8&amp;"',"&amp;C8&amp;")"&amp;IF(LEN(A9)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(7,'Brett Rypien',1),</v>
       </c>
       <c r="I8" s="9"/>
@@ -4097,7 +4097,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="str">
-        <f>"("&amp;A9&amp;",'"&amp;B9&amp;"',"&amp;C9&amp;")"&amp;IF(LEN(A10)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(8,'Brian Hoyer',1),</v>
       </c>
       <c r="I9" s="9"/>
@@ -4116,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="str">
-        <f>"("&amp;A10&amp;",'"&amp;B10&amp;"',"&amp;C10&amp;")"&amp;IF(LEN(A11)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(9,'Bryce Perkins',1),</v>
       </c>
       <c r="I10" s="9"/>
@@ -4135,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <f>"("&amp;A11&amp;",'"&amp;B11&amp;"',"&amp;C11&amp;")"&amp;IF(LEN(A12)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(10,'Cam Newton',1),</v>
       </c>
       <c r="I11" s="9"/>
@@ -4154,7 +4154,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <f>"("&amp;A12&amp;",'"&amp;B12&amp;"',"&amp;C12&amp;")"&amp;IF(LEN(A13)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(11,'Carson Wentz',1),</v>
       </c>
       <c r="I12" s="9"/>
@@ -4173,7 +4173,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <f>"("&amp;A13&amp;",'"&amp;B13&amp;"',"&amp;C13&amp;")"&amp;IF(LEN(A14)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(12,'Case Keenum',1),</v>
       </c>
       <c r="I13" s="9"/>
@@ -4192,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <f>"("&amp;A14&amp;",'"&amp;B14&amp;"',"&amp;C14&amp;")"&amp;IF(LEN(A15)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(13,'Chad Henne',1),</v>
       </c>
       <c r="I14" s="9"/>
@@ -4211,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f>"("&amp;A15&amp;",'"&amp;B15&amp;"',"&amp;C15&amp;")"&amp;IF(LEN(A16)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(14,'Chase Daniel',1),</v>
       </c>
       <c r="I15" s="9"/>
@@ -4230,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="str">
-        <f>"("&amp;A16&amp;",'"&amp;B16&amp;"',"&amp;C16&amp;")"&amp;IF(LEN(A17)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(15,'Colt McCoy',1),</v>
       </c>
       <c r="I16" s="9"/>
@@ -4249,7 +4249,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="str">
-        <f>"("&amp;A17&amp;",'"&amp;B17&amp;"',"&amp;C17&amp;")"&amp;IF(LEN(A18)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(16,'Cooper Rush',1),</v>
       </c>
       <c r="I17" s="9"/>
@@ -4268,7 +4268,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="str">
-        <f>"("&amp;A18&amp;",'"&amp;B18&amp;"',"&amp;C18&amp;")"&amp;IF(LEN(A19)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(17,'Dak Prescott',1),</v>
       </c>
       <c r="I18" s="9"/>
@@ -4287,7 +4287,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="str">
-        <f>"("&amp;A19&amp;",'"&amp;B19&amp;"',"&amp;C19&amp;")"&amp;IF(LEN(A20)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(18,'Daniel Jones',1),</v>
       </c>
       <c r="I19" s="9"/>
@@ -4306,7 +4306,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="str">
-        <f>"("&amp;A20&amp;",'"&amp;B20&amp;"',"&amp;C20&amp;")"&amp;IF(LEN(A21)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(19,'David Blough',1),</v>
       </c>
       <c r="I20" s="9"/>
@@ -4325,7 +4325,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="str">
-        <f>"("&amp;A21&amp;",'"&amp;B21&amp;"',"&amp;C21&amp;")"&amp;IF(LEN(A22)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(20,'Davis Mills',1),</v>
       </c>
       <c r="I21" s="9"/>
@@ -4344,7 +4344,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="str">
-        <f>"("&amp;A22&amp;",'"&amp;B22&amp;"',"&amp;C22&amp;")"&amp;IF(LEN(A23)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(21,'Derek Carr',1),</v>
       </c>
       <c r="I22" s="9"/>
@@ -4363,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="str">
-        <f>"("&amp;A23&amp;",'"&amp;B23&amp;"',"&amp;C23&amp;")"&amp;IF(LEN(A24)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(22,'Deshaun Watson',1),</v>
       </c>
       <c r="I23" s="9"/>
@@ -4382,7 +4382,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="str">
-        <f>"("&amp;A24&amp;",'"&amp;B24&amp;"',"&amp;C24&amp;")"&amp;IF(LEN(A25)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(23,'Drew Lock',1),</v>
       </c>
       <c r="I24" s="9"/>
@@ -4401,7 +4401,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="str">
-        <f>"("&amp;A25&amp;",'"&amp;B25&amp;"',"&amp;C25&amp;")"&amp;IF(LEN(A26)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(24,'Dwayne Haskins',0),</v>
       </c>
       <c r="I25" s="9"/>
@@ -4420,7 +4420,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="str">
-        <f>"("&amp;A26&amp;",'"&amp;B26&amp;"',"&amp;C26&amp;")"&amp;IF(LEN(A27)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(25,'Easton Stick',1),</v>
       </c>
       <c r="I26" s="9"/>
@@ -4439,7 +4439,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="str">
-        <f>"("&amp;A27&amp;",'"&amp;B27&amp;"',"&amp;C27&amp;")"&amp;IF(LEN(A28)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(26,'Feleipe Franks',1),</v>
       </c>
       <c r="I27" s="9"/>
@@ -4458,7 +4458,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="str">
-        <f>"("&amp;A28&amp;",'"&amp;B28&amp;"',"&amp;C28&amp;")"&amp;IF(LEN(A29)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(27,'Gardner Minshew',1),</v>
       </c>
       <c r="I28" s="9"/>
@@ -4477,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="str">
-        <f>"("&amp;A29&amp;",'"&amp;B29&amp;"',"&amp;C29&amp;")"&amp;IF(LEN(A30)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(28,'Garrett Gilbert',1),</v>
       </c>
       <c r="I29" s="9"/>
@@ -4496,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="str">
-        <f>"("&amp;A30&amp;",'"&amp;B30&amp;"',"&amp;C30&amp;")"&amp;IF(LEN(A31)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(29,'Geno Smith',1),</v>
       </c>
       <c r="I30" s="9"/>
@@ -4515,7 +4515,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="str">
-        <f>"("&amp;A31&amp;",'"&amp;B31&amp;"',"&amp;C31&amp;")"&amp;IF(LEN(A32)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(30,'Ian Book',1),</v>
       </c>
       <c r="I31" s="9"/>
@@ -4534,7 +4534,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="str">
-        <f>"("&amp;A32&amp;",'"&amp;B32&amp;"',"&amp;C32&amp;")"&amp;IF(LEN(A33)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(31,'Jacob Eason',1),</v>
       </c>
       <c r="I32" s="9"/>
@@ -4553,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="str">
-        <f>"("&amp;A33&amp;",'"&amp;B33&amp;"',"&amp;C33&amp;")"&amp;IF(LEN(A34)&gt;0,",","")</f>
+        <f t="shared" si="0"/>
         <v>(32,'Jacoby Brissett',1),</v>
       </c>
       <c r="I33" s="9"/>
@@ -4572,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="str">
-        <f>"("&amp;A34&amp;",'"&amp;B34&amp;"',"&amp;C34&amp;")"&amp;IF(LEN(A35)&gt;0,",","")</f>
+        <f t="shared" ref="E34:E65" si="1">"("&amp;A34&amp;",'"&amp;B34&amp;"',"&amp;C34&amp;")"&amp;IF(LEN(A35)&gt;0,",","")</f>
         <v>(33,'Jake Fromm',1),</v>
       </c>
       <c r="I34" s="9"/>
@@ -4591,7 +4591,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="str">
-        <f>"("&amp;A35&amp;",'"&amp;B35&amp;"',"&amp;C35&amp;")"&amp;IF(LEN(A36)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(34,'Jalen Hurts',1),</v>
       </c>
       <c r="I35" s="9"/>
@@ -4610,7 +4610,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="str">
-        <f>"("&amp;A36&amp;",'"&amp;B36&amp;"',"&amp;C36&amp;")"&amp;IF(LEN(A37)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(35,'Jameis Winston',1),</v>
       </c>
       <c r="I36" s="9"/>
@@ -4629,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="str">
-        <f>"("&amp;A37&amp;",'"&amp;B37&amp;"',"&amp;C37&amp;")"&amp;IF(LEN(A38)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(36,'Jared Goff',1),</v>
       </c>
       <c r="I37" s="9"/>
@@ -4648,7 +4648,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="str">
-        <f>"("&amp;A38&amp;",'"&amp;B38&amp;"',"&amp;C38&amp;")"&amp;IF(LEN(A39)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(37,'Jarrett Stidham',1),</v>
       </c>
       <c r="I38" s="9"/>
@@ -4667,7 +4667,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="str">
-        <f>"("&amp;A39&amp;",'"&amp;B39&amp;"',"&amp;C39&amp;")"&amp;IF(LEN(A40)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(38,'Jimmy Garoppolo',1),</v>
       </c>
       <c r="I39" s="9"/>
@@ -4686,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="str">
-        <f>"("&amp;A40&amp;",'"&amp;B40&amp;"',"&amp;C40&amp;")"&amp;IF(LEN(A41)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(39,'Joe Burrow',1),</v>
       </c>
       <c r="I40" s="9"/>
@@ -4705,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="str">
-        <f>"("&amp;A41&amp;",'"&amp;B41&amp;"',"&amp;C41&amp;")"&amp;IF(LEN(A42)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(40,'Joe Flacco',1),</v>
       </c>
       <c r="I41" s="9"/>
@@ -4724,7 +4724,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="str">
-        <f>"("&amp;A42&amp;",'"&amp;B42&amp;"',"&amp;C42&amp;")"&amp;IF(LEN(A43)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(41,'John Wolford',1),</v>
       </c>
       <c r="I42" s="9"/>
@@ -4743,7 +4743,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="str">
-        <f>"("&amp;A43&amp;",'"&amp;B43&amp;"',"&amp;C43&amp;")"&amp;IF(LEN(A44)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(42,'Jordan Love',1),</v>
       </c>
       <c r="I43" s="9"/>
@@ -4762,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="E44" t="str">
-        <f>"("&amp;A44&amp;",'"&amp;B44&amp;"',"&amp;C44&amp;")"&amp;IF(LEN(A45)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(43,'Josh Allen',1),</v>
       </c>
       <c r="I44" s="9"/>
@@ -4781,7 +4781,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="str">
-        <f>"("&amp;A45&amp;",'"&amp;B45&amp;"',"&amp;C45&amp;")"&amp;IF(LEN(A46)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(44,'Josh Johnson',1),</v>
       </c>
       <c r="I45" s="9"/>
@@ -4800,7 +4800,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="str">
-        <f>"("&amp;A46&amp;",'"&amp;B46&amp;"',"&amp;C46&amp;")"&amp;IF(LEN(A47)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(45,'Josh Rosen',1),</v>
       </c>
       <c r="I46" s="9"/>
@@ -4819,7 +4819,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="str">
-        <f>"("&amp;A47&amp;",'"&amp;B47&amp;"',"&amp;C47&amp;")"&amp;IF(LEN(A48)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(46,'Justin Fields',1),</v>
       </c>
       <c r="I47" s="9"/>
@@ -4838,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="str">
-        <f>"("&amp;A48&amp;",'"&amp;B48&amp;"',"&amp;C48&amp;")"&amp;IF(LEN(A49)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(47,'Justin Herbert',1),</v>
       </c>
       <c r="I48" s="9"/>
@@ -4857,7 +4857,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="str">
-        <f>"("&amp;A49&amp;",'"&amp;B49&amp;"',"&amp;C49&amp;")"&amp;IF(LEN(A50)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(48,'Kellen Mond',1),</v>
       </c>
       <c r="I49" s="9"/>
@@ -4876,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="str">
-        <f>"("&amp;A50&amp;",'"&amp;B50&amp;"',"&amp;C50&amp;")"&amp;IF(LEN(A51)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(49,'Kirk Cousins',1),</v>
       </c>
       <c r="I50" s="9"/>
@@ -4895,7 +4895,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="str">
-        <f>"("&amp;A51&amp;",'"&amp;B51&amp;"',"&amp;C51&amp;")"&amp;IF(LEN(A52)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(50,'Kyle Allen',1),</v>
       </c>
       <c r="I51" s="9"/>
@@ -4914,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="str">
-        <f>"("&amp;A52&amp;",'"&amp;B52&amp;"',"&amp;C52&amp;")"&amp;IF(LEN(A53)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(51,'Kyle Trask',1),</v>
       </c>
       <c r="I52" s="9"/>
@@ -4933,7 +4933,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="str">
-        <f>"("&amp;A53&amp;",'"&amp;B53&amp;"',"&amp;C53&amp;")"&amp;IF(LEN(A54)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(52,'Kyler Murray',1),</v>
       </c>
       <c r="I53" s="9"/>
@@ -4952,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="str">
-        <f>"("&amp;A54&amp;",'"&amp;B54&amp;"',"&amp;C54&amp;")"&amp;IF(LEN(A55)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(53,'Lamar Jackson',1),</v>
       </c>
       <c r="I54" s="9"/>
@@ -4971,7 +4971,7 @@
         <v>1</v>
       </c>
       <c r="E55" t="str">
-        <f>"("&amp;A55&amp;",'"&amp;B55&amp;"',"&amp;C55&amp;")"&amp;IF(LEN(A56)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(54,'Logan Woodside',1),</v>
       </c>
       <c r="I55" s="9"/>
@@ -4990,7 +4990,7 @@
         <v>1</v>
       </c>
       <c r="E56" t="str">
-        <f>"("&amp;A56&amp;",'"&amp;B56&amp;"',"&amp;C56&amp;")"&amp;IF(LEN(A57)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(55,'Mac Jones',1),</v>
       </c>
       <c r="I56" s="9"/>
@@ -5009,7 +5009,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="str">
-        <f>"("&amp;A57&amp;",'"&amp;B57&amp;"',"&amp;C57&amp;")"&amp;IF(LEN(A58)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(56,'Marcus Mariota',1),</v>
       </c>
       <c r="I57" s="9"/>
@@ -5028,7 +5028,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="str">
-        <f>"("&amp;A58&amp;",'"&amp;B58&amp;"',"&amp;C58&amp;")"&amp;IF(LEN(A59)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(57,'Mason Rudolph',1),</v>
       </c>
       <c r="I58" s="9"/>
@@ -5047,7 +5047,7 @@
         <v>1</v>
       </c>
       <c r="E59" t="str">
-        <f>"("&amp;A59&amp;",'"&amp;B59&amp;"',"&amp;C59&amp;")"&amp;IF(LEN(A60)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(58,'Matt Ryan',1),</v>
       </c>
       <c r="I59" s="9"/>
@@ -5066,7 +5066,7 @@
         <v>1</v>
       </c>
       <c r="E60" t="str">
-        <f>"("&amp;A60&amp;",'"&amp;B60&amp;"',"&amp;C60&amp;")"&amp;IF(LEN(A61)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(59,'Matthew Stafford',1),</v>
       </c>
       <c r="I60" s="9"/>
@@ -5085,7 +5085,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="str">
-        <f>"("&amp;A61&amp;",'"&amp;B61&amp;"',"&amp;C61&amp;")"&amp;IF(LEN(A62)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(60,'Mike Glennon',1),</v>
       </c>
       <c r="I61" s="9"/>
@@ -5104,7 +5104,7 @@
         <v>1</v>
       </c>
       <c r="E62" t="str">
-        <f>"("&amp;A62&amp;",'"&amp;B62&amp;"',"&amp;C62&amp;")"&amp;IF(LEN(A63)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(61,'Mike White',1),</v>
       </c>
       <c r="I62" s="9"/>
@@ -5123,7 +5123,7 @@
         <v>1</v>
       </c>
       <c r="E63" t="str">
-        <f>"("&amp;A63&amp;",'"&amp;B63&amp;"',"&amp;C63&amp;")"&amp;IF(LEN(A64)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(62,'Mitchell Trubisky',1),</v>
       </c>
       <c r="I63" s="9"/>
@@ -5142,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="E64" t="str">
-        <f>"("&amp;A64&amp;",'"&amp;B64&amp;"',"&amp;C64&amp;")"&amp;IF(LEN(A65)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(63,'Nick Foles',1),</v>
       </c>
       <c r="I64" s="9"/>
@@ -5161,7 +5161,7 @@
         <v>1</v>
       </c>
       <c r="E65" t="str">
-        <f>"("&amp;A65&amp;",'"&amp;B65&amp;"',"&amp;C65&amp;")"&amp;IF(LEN(A66)&gt;0,",","")</f>
+        <f t="shared" si="1"/>
         <v>(64,'Nick Mullens',1),</v>
       </c>
       <c r="I65" s="9"/>
@@ -5180,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="E66" t="str">
-        <f>"("&amp;A66&amp;",'"&amp;B66&amp;"',"&amp;C66&amp;")"&amp;IF(LEN(A67)&gt;0,",","")</f>
+        <f t="shared" ref="E66:E94" si="2">"("&amp;A66&amp;",'"&amp;B66&amp;"',"&amp;C66&amp;")"&amp;IF(LEN(A67)&gt;0,",","")</f>
         <v>(65,'PJ Walker',1),</v>
       </c>
       <c r="I66" s="9"/>
@@ -5199,7 +5199,7 @@
         <v>1</v>
       </c>
       <c r="E67" t="str">
-        <f>"("&amp;A67&amp;",'"&amp;B67&amp;"',"&amp;C67&amp;")"&amp;IF(LEN(A68)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(66,'Patrick Mahomes',1),</v>
       </c>
       <c r="I67" s="9"/>
@@ -5218,7 +5218,7 @@
         <v>1</v>
       </c>
       <c r="E68" t="str">
-        <f>"("&amp;A68&amp;",'"&amp;B68&amp;"',"&amp;C68&amp;")"&amp;IF(LEN(A69)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(67,'Reid Sinnett',1),</v>
       </c>
       <c r="I68" s="9"/>
@@ -5237,7 +5237,7 @@
         <v>1</v>
       </c>
       <c r="E69" t="str">
-        <f>"("&amp;A69&amp;",'"&amp;B69&amp;"',"&amp;C69&amp;")"&amp;IF(LEN(A70)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(68,'Russell Wilson',1),</v>
       </c>
       <c r="I69" s="9"/>
@@ -5256,7 +5256,7 @@
         <v>1</v>
       </c>
       <c r="E70" t="str">
-        <f>"("&amp;A70&amp;",'"&amp;B70&amp;"',"&amp;C70&amp;")"&amp;IF(LEN(A71)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(69,'Ryan Tannehill',1),</v>
       </c>
       <c r="I70" s="9"/>
@@ -5275,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="E71" t="str">
-        <f>"("&amp;A71&amp;",'"&amp;B71&amp;"',"&amp;C71&amp;")"&amp;IF(LEN(A72)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(70,'Sam Darnold',1),</v>
       </c>
       <c r="I71" s="9"/>
@@ -5294,7 +5294,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="str">
-        <f>"("&amp;A72&amp;",'"&amp;B72&amp;"',"&amp;C72&amp;")"&amp;IF(LEN(A73)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(71,'Sam Ehlinger',1),</v>
       </c>
       <c r="I72" s="9"/>
@@ -5313,7 +5313,7 @@
         <v>1</v>
       </c>
       <c r="E73" t="str">
-        <f>"("&amp;A73&amp;",'"&amp;B73&amp;"',"&amp;C73&amp;")"&amp;IF(LEN(A74)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(72,'Sean Mannion',1),</v>
       </c>
       <c r="I73" s="9"/>
@@ -5332,7 +5332,7 @@
         <v>1</v>
       </c>
       <c r="E74" t="str">
-        <f>"("&amp;A74&amp;",'"&amp;B74&amp;"',"&amp;C74&amp;")"&amp;IF(LEN(A75)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(73,'Shane Buechele',1),</v>
       </c>
       <c r="I74" s="9"/>
@@ -5351,7 +5351,7 @@
         <v>1</v>
       </c>
       <c r="E75" t="str">
-        <f>"("&amp;A75&amp;",'"&amp;B75&amp;"',"&amp;C75&amp;")"&amp;IF(LEN(A76)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(74,'Taylor Heinicke',1),</v>
       </c>
       <c r="I75" s="9"/>
@@ -5370,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="E76" t="str">
-        <f>"("&amp;A76&amp;",'"&amp;B76&amp;"',"&amp;C76&amp;")"&amp;IF(LEN(A77)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(75,'Taysom Hill',1),</v>
       </c>
       <c r="I76" s="9"/>
@@ -5389,7 +5389,7 @@
         <v>1</v>
       </c>
       <c r="E77" t="str">
-        <f>"("&amp;A77&amp;",'"&amp;B77&amp;"',"&amp;C77&amp;")"&amp;IF(LEN(A78)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(76,'Teddy Bridgewater',1),</v>
       </c>
       <c r="I77" s="9"/>
@@ -5408,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="E78" t="str">
-        <f>"("&amp;A78&amp;",'"&amp;B78&amp;"',"&amp;C78&amp;")"&amp;IF(LEN(A79)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(77,'Tim Boyle',1),</v>
       </c>
       <c r="I78" s="9"/>
@@ -5427,7 +5427,7 @@
         <v>1</v>
       </c>
       <c r="E79" t="str">
-        <f>"("&amp;A79&amp;",'"&amp;B79&amp;"',"&amp;C79&amp;")"&amp;IF(LEN(A80)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(78,'Tom Brady',1),</v>
       </c>
       <c r="I79" s="9"/>
@@ -5446,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="E80" t="str">
-        <f>"("&amp;A80&amp;",'"&amp;B80&amp;"',"&amp;C80&amp;")"&amp;IF(LEN(A81)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(79,'Trace McSorley',1),</v>
       </c>
       <c r="I80" s="9"/>
@@ -5465,7 +5465,7 @@
         <v>1</v>
       </c>
       <c r="E81" t="str">
-        <f>"("&amp;A81&amp;",'"&amp;B81&amp;"',"&amp;C81&amp;")"&amp;IF(LEN(A82)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(80,'Trevor Lawrence',1),</v>
       </c>
       <c r="I81" s="9"/>
@@ -5484,7 +5484,7 @@
         <v>1</v>
       </c>
       <c r="E82" t="str">
-        <f>"("&amp;A82&amp;",'"&amp;B82&amp;"',"&amp;C82&amp;")"&amp;IF(LEN(A83)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(81,'Trevor Siemian',1),</v>
       </c>
       <c r="I82" s="9"/>
@@ -5503,7 +5503,7 @@
         <v>1</v>
       </c>
       <c r="E83" t="str">
-        <f>"("&amp;A83&amp;",'"&amp;B83&amp;"',"&amp;C83&amp;")"&amp;IF(LEN(A84)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(82,'Trey Lance',1),</v>
       </c>
       <c r="I83" s="9"/>
@@ -5522,7 +5522,7 @@
         <v>1</v>
       </c>
       <c r="E84" t="str">
-        <f>"("&amp;A84&amp;",'"&amp;B84&amp;"',"&amp;C84&amp;")"&amp;IF(LEN(A85)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(83,'Tua Tagovailoa',1),</v>
       </c>
       <c r="I84" s="9"/>
@@ -5541,7 +5541,7 @@
         <v>1</v>
       </c>
       <c r="E85" t="str">
-        <f>"("&amp;A85&amp;",'"&amp;B85&amp;"',"&amp;C85&amp;")"&amp;IF(LEN(A86)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(84,'Tyler Huntley',1),</v>
       </c>
       <c r="I85" s="9"/>
@@ -5560,7 +5560,7 @@
         <v>1</v>
       </c>
       <c r="E86" t="str">
-        <f>"("&amp;A86&amp;",'"&amp;B86&amp;"',"&amp;C86&amp;")"&amp;IF(LEN(A87)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(85,'Tyrod Taylor',1),</v>
       </c>
       <c r="I86" s="9"/>
@@ -5579,7 +5579,7 @@
         <v>1</v>
       </c>
       <c r="E87" t="str">
-        <f>"("&amp;A87&amp;",'"&amp;B87&amp;"',"&amp;C87&amp;")"&amp;IF(LEN(A88)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(86,'Zach Wilson',1),</v>
       </c>
       <c r="I87" s="9"/>
@@ -5598,7 +5598,7 @@
         <v>1</v>
       </c>
       <c r="E88" t="str">
-        <f>"("&amp;A88&amp;",'"&amp;B88&amp;"',"&amp;C88&amp;")"&amp;IF(LEN(A89)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(87,'Bailey Zappe',1),</v>
       </c>
       <c r="I88" s="9"/>
@@ -5617,7 +5617,7 @@
         <v>1</v>
       </c>
       <c r="E89" t="str">
-        <f>"("&amp;A89&amp;",'"&amp;B89&amp;"',"&amp;C89&amp;")"&amp;IF(LEN(A90)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(88,'Carson Strong',1),</v>
       </c>
       <c r="I89" s="9"/>
@@ -5636,7 +5636,7 @@
         <v>1</v>
       </c>
       <c r="E90" t="str">
-        <f>"("&amp;A90&amp;",'"&amp;B90&amp;"',"&amp;C90&amp;")"&amp;IF(LEN(A91)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(89,'Desmond Ridder',1),</v>
       </c>
       <c r="I90" s="9"/>
@@ -5655,7 +5655,7 @@
         <v>1</v>
       </c>
       <c r="E91" t="str">
-        <f>"("&amp;A91&amp;",'"&amp;B91&amp;"',"&amp;C91&amp;")"&amp;IF(LEN(A92)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(90,'Kenny Pickett',1),</v>
       </c>
       <c r="I91" s="9"/>
@@ -5674,7 +5674,7 @@
         <v>1</v>
       </c>
       <c r="E92" t="str">
-        <f>"("&amp;A92&amp;",'"&amp;B92&amp;"',"&amp;C92&amp;")"&amp;IF(LEN(A93)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(91,'Malik Willis',1),</v>
       </c>
       <c r="I92" s="9"/>
@@ -5693,7 +5693,7 @@
         <v>1</v>
       </c>
       <c r="E93" t="str">
-        <f>"("&amp;A93&amp;",'"&amp;B93&amp;"',"&amp;C93&amp;")"&amp;IF(LEN(A94)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(92,'Matt Corral',1),</v>
       </c>
       <c r="I93" s="9"/>
@@ -5712,7 +5712,7 @@
         <v>1</v>
       </c>
       <c r="E94" t="str">
-        <f>"("&amp;A94&amp;",'"&amp;B94&amp;"',"&amp;C94&amp;")"&amp;IF(LEN(A95)&gt;0,",","")</f>
+        <f t="shared" si="2"/>
         <v>(93,'Sam Howell',1),</v>
       </c>
       <c r="I94" s="9"/>
@@ -5731,7 +5731,7 @@
         <v>1</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" ref="E95:E105" si="0">"("&amp;A95&amp;",'"&amp;B95&amp;"',"&amp;C95&amp;")"&amp;IF(LEN(A96)&gt;0,",","")</f>
+        <f t="shared" ref="E95:E105" si="3">"("&amp;A95&amp;",'"&amp;B95&amp;"',"&amp;C95&amp;")"&amp;IF(LEN(A96)&gt;0,",","")</f>
         <v>(94,'Bryce Young',1),</v>
       </c>
       <c r="I95" s="9"/>
@@ -5750,7 +5750,7 @@
         <v>1</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(95,'CJ Stroud',1),</v>
       </c>
     </row>
@@ -5765,7 +5765,7 @@
         <v>1</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(96,'Will Levis',1),</v>
       </c>
     </row>
@@ -5780,7 +5780,7 @@
         <v>1</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(97,'Hendon Hooker',1),</v>
       </c>
     </row>
@@ -5795,7 +5795,7 @@
         <v>1</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(98,'Anthony Richardson',1),</v>
       </c>
     </row>
@@ -5810,7 +5810,7 @@
         <v>1</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(99,'Tyler Van Dyke',1),</v>
       </c>
     </row>
@@ -5825,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(100,'Tanner McKee',1),</v>
       </c>
     </row>
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(101,'KJ Jefferson',1),</v>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
         <v>1</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(102,'Jaren Hall',1),</v>
       </c>
     </row>
@@ -5870,7 +5870,7 @@
         <v>1</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(103,'Jayden Daniels',1),</v>
       </c>
     </row>
@@ -5885,7 +5885,7 @@
         <v>1</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>(104,'Malik Cunningham',1)</v>
       </c>
     </row>
@@ -6293,8 +6293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I1:I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cleaned up outside prediction period page
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771B0897-7FA7-4478-AE68-662D1C28DD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAAC270-1617-4D06-B914-D21CF8331CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="282">
   <si>
     <t>TeamID</t>
   </si>
@@ -905,6 +905,21 @@
   </si>
   <si>
     <t>DefaultPlayerID</t>
+  </si>
+  <si>
+    <t>KO of 2023 Regular Season opener</t>
+  </si>
+  <si>
+    <t>KO of 1st game in final round of 2023 Regular Season games</t>
+  </si>
+  <si>
+    <t>Start of 2024 League Year and Free Agency</t>
+  </si>
+  <si>
+    <t>Start of 2024 NFL Draft</t>
+  </si>
+  <si>
+    <t>KO of Super Bowl LVIII</t>
   </si>
 </sst>
 </file>
@@ -6293,7 +6308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -6558,10 +6573,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F502399-C795-4D5E-88DC-92C8B5181153}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F1:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6622,7 +6637,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F11" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"',"&amp;IF(LEN(C3)&gt;0,"'"&amp;TEXT(C3,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <f t="shared" ref="F3:F16" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"',"&amp;IF(LEN(C3)&gt;0,"'"&amp;TEXT(C3,"YYYY-MM-DD HH:MM")&amp;"'","NULL")&amp;","&amp;D3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
         <v>(2,'KO of 1st game in final round of 2021 Regular Season games','2022-01-08 21:30',1),</v>
       </c>
     </row>
@@ -6673,11 +6688,11 @@
         <v>44680</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>(5,'Start of 2022 NFL Draft','2022-04-29 00:00',0),</v>
+        <v>(5,'Start of 2022 NFL Draft','2022-04-29 00:00',1),</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -6691,11 +6706,11 @@
         <v>44813.013888888891</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>(6,'KO of 2022 Regular Season opener','2022-09-09 00:20',0),</v>
+        <v>(6,'KO of 2022 Regular Season opener','2022-09-09 00:20',1),</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -6727,11 +6742,11 @@
         <v>44969.979166666664</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>(8,'KO of Super Bowl LVII','2023-02-12 23:30',0),</v>
+        <v>(8,'KO of Super Bowl LVII','2023-02-12 23:30',1),</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -6745,11 +6760,11 @@
         <v>45000.833333333336</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>(9,'Start of 2023 League Year and Free Agency','2023-03-15 20:00',0),</v>
+        <v>(9,'Start of 2023 League Year and Free Agency','2023-03-15 20:00',1),</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -6763,23 +6778,101 @@
         <v>45044</v>
       </c>
       <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,'Start of 2023 NFL Draft','2023-04-28 00:00',1),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45177.013888888891</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>(10,'Start of 2023 NFL Draft','2023-04-28 00:00',0)</v>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,'KO of 2023 Regular Season opener','2023-09-08 00:20',0),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45298.895833333336</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,'KO of 1st game in final round of 2023 Regular Season games','2024-01-07 21:30',0),</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" t="str">
-        <f>YEAR(C2)&amp;"-"&amp;MONTH(C2)&amp;"-"&amp;DAY(C2)</f>
-        <v>2021-9-10</v>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45333.979166666664</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,'KO of Super Bowl LVIII','2024-02-11 23:30',0),</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" t="str">
-        <f>TEXT(C2,"YYYY-MM-DD HH:MM")</f>
-        <v>2021-09-10 00:20</v>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45365.833333333336</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,'Start of 2024 League Year and Free Agency','2024-03-14 20:00',0),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45408</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,'Start of 2024 NFL Draft','2024-04-26 00:00',0)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started looking at leaderboards
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAAC270-1617-4D06-B914-D21CF8331CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE0B66-147F-4FB0-89F2-F91371BD9EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="283">
   <si>
     <t>TeamID</t>
   </si>
@@ -920,6 +920,9 @@
   </si>
   <si>
     <t>KO of Super Bowl LVIII</t>
+  </si>
+  <si>
+    <t>IsSeasonTotal</t>
   </si>
 </sst>
 </file>
@@ -6306,10 +6309,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E88BF7-FA4B-4AC8-BFBD-81561F4F3A4F}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6322,7 +6325,7 @@
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>82</v>
       </c>
@@ -6344,12 +6347,15 @@
       <c r="G1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I1" t="str" cm="1">
-        <f t="array" aca="1" ref="I1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:G1)&amp;") VALUES"</f>
-        <v>INSERT INTO the_qb_carousel.PredictionPeriods(PredictionPeriodID,Season,SeasonPeriodID,FromEventID,ToEventID,HowItWorks,IsActive) VALUES</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J1" t="str" cm="1">
+        <f t="array" aca="1" ref="J1" ca="1">"INSERT INTO the_qb_carousel."&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;"("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:H1)&amp;") VALUES"</f>
+        <v>INSERT INTO the_qb_carousel.PredictionPeriods(PredictionPeriodID,Season,SeasonPeriodID,FromEventID,ToEventID,HowItWorks,IsActive,IsSeasonTotal) VALUES</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6371,12 +6377,15 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2" t="str">
-        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"',"&amp;F2&amp;","&amp;G2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
-        <v>('1',2022,'1','1','2',1,1),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"('"&amp;A2&amp;"',"&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"',"&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
+        <v>('1',2022,'1','1','2',1,1,0),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6398,12 +6407,15 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I9" si="0">"('"&amp;A3&amp;"',"&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"',"&amp;F3&amp;","&amp;G3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
-        <v>('2',2022,'2','2','3',1,1),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J9" si="0">"('"&amp;A3&amp;"',"&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"',"&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;")"&amp;IF(LEN(A4)&gt;0,",","")</f>
+        <v>('2',2022,'2','2','3',1,1,0),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6425,12 +6437,15 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>('3',2022,'3','3','4',1,1),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>('3',2022,'3','3','4',1,1,0),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6452,12 +6467,15 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>('4',2022,'4','4','5',1,1),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>('4',2022,'4','4','5',1,1,0),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6479,12 +6497,15 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>('5',2023,'1','6','7',0,1),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>('5',2023,'1','6','7',0,1,0),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6506,12 +6527,15 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>('6',2023,'2','7','8',0,1),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>('6',2023,'2','7','8',0,1,0),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6533,12 +6557,15 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>('7',2023,'3','8','9',0,1),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>('7',2023,'3','8','9',0,1,0),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6560,9 +6587,12 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>('8',2023,'4','9','10',0,1)</v>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>('8',2023,'4','9','10',0,1,0)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Good progress on global leaderboard
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE0B66-147F-4FB0-89F2-F91371BD9EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681E777B-A1B1-4FC2-8BC8-210194DF9CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="284">
   <si>
     <t>TeamID</t>
   </si>
@@ -923,13 +923,16 @@
   </si>
   <si>
     <t>IsSeasonTotal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO UserScores (UserID,PredictionPeriodID,Score) VALUES </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,6 +970,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -994,7 +1003,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1008,6 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1400,13 +1409,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1446,7 +1455,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1476,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AAA072-D9CC-49CB-9957-A9B3539B4826}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1485,7 +1494,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1569,10 +1578,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1615,10 +1624,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,26 +1635,1668 @@
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2">
+      <c r="D1" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"("&amp;A2&amp;","&amp;B2&amp;","&amp;C2&amp;"),"</f>
+        <v>(2,1,0.0625),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="0">"("&amp;A3&amp;","&amp;B3&amp;","&amp;C3&amp;"),"</f>
+        <v>(2,2,0.46875),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>(2,3,0.03125),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.34375</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>(2,4,0.34375),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.2265625</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>(2,1234,0.2265625),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.78125</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,1,0.78125),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.1875</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,2,0.1875),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,4,0.90625),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,1234,0.46875),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,1,0.9375),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,2,0.125),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.34375</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,3,0.34375),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>4</v>
+      </c>
+      <c r="B14" s="9">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.96875</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,4,0.96875),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.59375</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,1234,0.59375),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
         <v>0.875</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,1,0.875),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>4</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,4,0.03125),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>5</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.2265625</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,1234,0.2265625),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
+        <v>6</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.3125</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,1,0.3125),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>6</v>
+      </c>
+      <c r="B20" s="9">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.84375</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,2,0.84375),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>6</v>
+      </c>
+      <c r="B21" s="9">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.9375</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,3,0.9375),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
+        <v>6</v>
+      </c>
+      <c r="B22" s="9">
+        <v>4</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,4,0.5625),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
+        <v>6</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.6640625</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,1234,0.6640625),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,1,0.5),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
+        <v>7</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.59375</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,2,0.59375),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
+        <v>7</v>
+      </c>
+      <c r="B26" s="9">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,3,0.90625),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>7</v>
+      </c>
+      <c r="B27" s="9">
+        <v>4</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,4,0.90625),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>7</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.7265625</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,1234,0.7265625),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
+        <v>8</v>
+      </c>
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.40625</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,1,0.40625),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
+        <v>8</v>
+      </c>
+      <c r="B30" s="9">
+        <v>2</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.21875</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,2,0.21875),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
+        <v>8</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.15625</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,1234,0.15625),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
+        <v>9</v>
+      </c>
+      <c r="B32" s="9">
+        <v>1</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,1,0.90625),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>9</v>
+      </c>
+      <c r="B33" s="9">
+        <v>2</v>
+      </c>
+      <c r="C33" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,2,0.0625),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="9">
+        <v>9</v>
+      </c>
+      <c r="B34" s="9">
+        <v>3</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0.3125</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,3,0.3125),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>9</v>
+      </c>
+      <c r="B35" s="9">
+        <v>4</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,4,0.46875),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
+        <v>9</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0.4375</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,1234,0.4375),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>10</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0.34375</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,1,0.34375),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>10</v>
+      </c>
+      <c r="B38" s="9">
+        <v>2</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,2,0.625),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="9">
+        <v>10</v>
+      </c>
+      <c r="B39" s="9">
+        <v>4</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,4,0.46875),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="9">
+        <v>10</v>
+      </c>
+      <c r="B40" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.359375</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,1234,0.359375),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
+        <v>11</v>
+      </c>
+      <c r="B41" s="9">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9">
+        <v>0.15625</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,1,0.15625),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
+        <v>11</v>
+      </c>
+      <c r="B42" s="9">
+        <v>2</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0.34375</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,2,0.34375),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
+        <v>11</v>
+      </c>
+      <c r="B43" s="9">
+        <v>3</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,3,0.46875),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
+        <v>11</v>
+      </c>
+      <c r="B44" s="9">
+        <v>4</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,4,0.6875),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
+        <v>11</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0.4140625</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,1234,0.4140625),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="9">
+        <v>12</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,1,0.5),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
+        <v>12</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.84375</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,2,0.84375),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="9">
+        <v>12</v>
+      </c>
+      <c r="B48" s="9">
+        <v>3</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,3,0.53125),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="9">
+        <v>12</v>
+      </c>
+      <c r="B49" s="9">
+        <v>4</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0.59375</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,4,0.59375),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
+        <v>12</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.6171875</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,1234,0.6171875),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
+        <v>13</v>
+      </c>
+      <c r="B51" s="9">
+        <v>2</v>
+      </c>
+      <c r="C51" s="9">
+        <v>0.4375</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,2,0.4375),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="9">
+        <v>13</v>
+      </c>
+      <c r="B52" s="9">
+        <v>3</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,3,0),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
+        <v>13</v>
+      </c>
+      <c r="B53" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.109375</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,1234,0.109375),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="9">
+        <v>14</v>
+      </c>
+      <c r="B54" s="9">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,1,0.53125),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="9">
+        <v>14</v>
+      </c>
+      <c r="B55" s="9">
+        <v>2</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.3125</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,2,0.3125),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="9">
+        <v>14</v>
+      </c>
+      <c r="B56" s="9">
+        <v>3</v>
+      </c>
+      <c r="C56" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,3,0.375),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="9">
+        <v>14</v>
+      </c>
+      <c r="B57" s="9">
+        <v>4</v>
+      </c>
+      <c r="C57" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,4,0.875),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="9">
+        <v>14</v>
+      </c>
+      <c r="B58" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0.5234375</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,1234,0.5234375),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="9">
+        <v>15</v>
+      </c>
+      <c r="B59" s="9">
+        <v>2</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.96875</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,2,0.96875),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="9">
+        <v>15</v>
+      </c>
+      <c r="B60" s="9">
+        <v>3</v>
+      </c>
+      <c r="C60" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,3,0.6875),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="9">
+        <v>15</v>
+      </c>
+      <c r="B61" s="9">
+        <v>4</v>
+      </c>
+      <c r="C61" s="9">
+        <v>0.8125</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,4,0.8125),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="9">
+        <v>15</v>
+      </c>
+      <c r="B62" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0.6171875</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,1234,0.6171875),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="9">
+        <v>16</v>
+      </c>
+      <c r="B63" s="9">
+        <v>1</v>
+      </c>
+      <c r="C63" s="9">
+        <v>0.40625</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,1,0.40625),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="9">
+        <v>16</v>
+      </c>
+      <c r="B64" s="9">
+        <v>2</v>
+      </c>
+      <c r="C64" s="9">
+        <v>0.8125</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,2,0.8125),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="9">
+        <v>16</v>
+      </c>
+      <c r="B65" s="9">
+        <v>3</v>
+      </c>
+      <c r="C65" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,3,0.75),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="9">
+        <v>16</v>
+      </c>
+      <c r="B66" s="9">
+        <v>4</v>
+      </c>
+      <c r="C66" s="9">
+        <v>0.21875</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,4,0.21875),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="9">
+        <v>16</v>
+      </c>
+      <c r="B67" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0.546875</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D111" si="1">"("&amp;A67&amp;","&amp;B67&amp;","&amp;C67&amp;"),"</f>
+        <v>(16,1234,0.546875),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="9">
+        <v>17</v>
+      </c>
+      <c r="B68" s="9">
+        <v>1</v>
+      </c>
+      <c r="C68" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>(17,1,0.03125),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="9">
+        <v>17</v>
+      </c>
+      <c r="B69" s="9">
+        <v>3</v>
+      </c>
+      <c r="C69" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>(17,3,0.5),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="9">
+        <v>17</v>
+      </c>
+      <c r="B70" s="9">
+        <v>4</v>
+      </c>
+      <c r="C70" s="9">
+        <v>0.65625</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>(17,4,0.65625),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="9">
+        <v>17</v>
+      </c>
+      <c r="B71" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.296875</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>(17,1234,0.296875),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="9">
+        <v>18</v>
+      </c>
+      <c r="B72" s="9">
+        <v>1</v>
+      </c>
+      <c r="C72" s="9">
+        <v>0.40625</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>(18,1,0.40625),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="9">
+        <v>18</v>
+      </c>
+      <c r="B73" s="9">
+        <v>2</v>
+      </c>
+      <c r="C73" s="9">
+        <v>0.40625</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>(18,2,0.40625),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="9">
+        <v>18</v>
+      </c>
+      <c r="B74" s="9">
+        <v>3</v>
+      </c>
+      <c r="C74" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>(18,3,0.125),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="9">
+        <v>18</v>
+      </c>
+      <c r="B75" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C75" s="9">
+        <v>0.234375</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>(18,1234,0.234375),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="9">
+        <v>19</v>
+      </c>
+      <c r="B76" s="9">
+        <v>1</v>
+      </c>
+      <c r="C76" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>(19,1,0.6875),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="9">
+        <v>19</v>
+      </c>
+      <c r="B77" s="9">
+        <v>2</v>
+      </c>
+      <c r="C77" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>(19,2,0.53125),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="9">
+        <v>19</v>
+      </c>
+      <c r="B78" s="9">
+        <v>3</v>
+      </c>
+      <c r="C78" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>(19,3,0.53125),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="9">
+        <v>19</v>
+      </c>
+      <c r="B79" s="9">
+        <v>4</v>
+      </c>
+      <c r="C79" s="9">
+        <v>0.65625</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>(19,4,0.65625),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="9">
+        <v>19</v>
+      </c>
+      <c r="B80" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C80" s="9">
+        <v>0.6015625</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>(19,1234,0.6015625),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="9">
+        <v>20</v>
+      </c>
+      <c r="B81" s="9">
+        <v>1</v>
+      </c>
+      <c r="C81" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>(20,1,0.25),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="9">
+        <v>20</v>
+      </c>
+      <c r="B82" s="9">
+        <v>3</v>
+      </c>
+      <c r="C82" s="9">
+        <v>0.90625</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>(20,3,0.90625),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="9">
+        <v>20</v>
+      </c>
+      <c r="B83" s="9">
+        <v>4</v>
+      </c>
+      <c r="C83" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>(20,4,0.03125),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="9">
+        <v>20</v>
+      </c>
+      <c r="B84" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C84" s="9">
+        <v>0.296875</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>(20,1234,0.296875),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="9">
+        <v>21</v>
+      </c>
+      <c r="B85" s="9">
+        <v>1</v>
+      </c>
+      <c r="C85" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>(21,1,0.125),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="9">
+        <v>21</v>
+      </c>
+      <c r="B86" s="9">
+        <v>2</v>
+      </c>
+      <c r="C86" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>(21,2,0.25),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="9">
+        <v>21</v>
+      </c>
+      <c r="B87" s="9">
+        <v>3</v>
+      </c>
+      <c r="C87" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>(21,3,0.625),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="9">
+        <v>21</v>
+      </c>
+      <c r="B88" s="9">
+        <v>4</v>
+      </c>
+      <c r="C88" s="9">
+        <v>0.5625</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>(21,4,0.5625),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="9">
+        <v>21</v>
+      </c>
+      <c r="B89" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C89" s="9">
+        <v>0.390625</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>(21,1234,0.390625),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="9">
+        <v>22</v>
+      </c>
+      <c r="B90" s="9">
+        <v>1</v>
+      </c>
+      <c r="C90" s="9">
+        <v>0.4375</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>(22,1,0.4375),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="9">
+        <v>22</v>
+      </c>
+      <c r="B91" s="9">
+        <v>2</v>
+      </c>
+      <c r="C91" s="9">
+        <v>0</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>(22,2,0),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="9">
+        <v>22</v>
+      </c>
+      <c r="B92" s="9">
+        <v>4</v>
+      </c>
+      <c r="C92" s="9">
+        <v>0.15625</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>(22,4,0.15625),</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="9">
+        <v>22</v>
+      </c>
+      <c r="B93" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C93" s="9">
+        <v>0.1484375</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>(22,1234,0.1484375),</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="9">
+        <v>23</v>
+      </c>
+      <c r="B94" s="9">
+        <v>2</v>
+      </c>
+      <c r="C94" s="9">
+        <v>0.53125</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>(23,2,0.53125),</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="9">
+        <v>23</v>
+      </c>
+      <c r="B95" s="9">
+        <v>3</v>
+      </c>
+      <c r="C95" s="9">
+        <v>0.46875</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>(23,3,0.46875),</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="9">
+        <v>23</v>
+      </c>
+      <c r="B96" s="9">
+        <v>4</v>
+      </c>
+      <c r="C96" s="9">
+        <v>0</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>(23,4,0),</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="9">
+        <v>23</v>
+      </c>
+      <c r="B97" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C97" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>(23,1234,0.25),</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="9">
+        <v>24</v>
+      </c>
+      <c r="B98" s="9">
+        <v>2</v>
+      </c>
+      <c r="C98" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>(24,2,0.125),</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="9">
+        <v>24</v>
+      </c>
+      <c r="B99" s="9">
+        <v>3</v>
+      </c>
+      <c r="C99" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>(24,3,0.5),</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="9">
+        <v>24</v>
+      </c>
+      <c r="B100" s="9">
+        <v>4</v>
+      </c>
+      <c r="C100" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>(24,4,0.6875),</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="9">
+        <v>24</v>
+      </c>
+      <c r="B101" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C101" s="9">
+        <v>0.328125</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>(24,1234,0.328125),</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="9">
+        <v>25</v>
+      </c>
+      <c r="B102" s="9">
+        <v>1</v>
+      </c>
+      <c r="C102" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>(25,1,0.0625),</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="9">
+        <v>25</v>
+      </c>
+      <c r="B103" s="9">
+        <v>2</v>
+      </c>
+      <c r="C103" s="9">
+        <v>0.78125</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>(25,2,0.78125),</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="9">
+        <v>25</v>
+      </c>
+      <c r="B104" s="9">
+        <v>3</v>
+      </c>
+      <c r="C104" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>(25,3,0.03125),</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="9">
+        <v>25</v>
+      </c>
+      <c r="B105" s="9">
+        <v>4</v>
+      </c>
+      <c r="C105" s="9">
+        <v>0.71875</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="1"/>
+        <v>(25,4,0.71875),</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="9">
+        <v>25</v>
+      </c>
+      <c r="B106" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C106" s="9">
+        <v>0.3984375</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>(25,1234,0.3984375),</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="9">
+        <v>26</v>
+      </c>
+      <c r="B107" s="9">
+        <v>1</v>
+      </c>
+      <c r="C107" s="9">
+        <v>0.84375</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>(26,1,0.84375),</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="9">
+        <v>26</v>
+      </c>
+      <c r="B108" s="9">
+        <v>2</v>
+      </c>
+      <c r="C108" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>(26,2,0.875),</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="9">
+        <v>26</v>
+      </c>
+      <c r="B109" s="9">
+        <v>3</v>
+      </c>
+      <c r="C109" s="9">
+        <v>0</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>(26,3,0),</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="9">
+        <v>26</v>
+      </c>
+      <c r="B110" s="9">
+        <v>4</v>
+      </c>
+      <c r="C110" s="9">
+        <v>0.1875</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>(26,4,0.1875),</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="9">
+        <v>26</v>
+      </c>
+      <c r="B111" s="9">
+        <v>1234</v>
+      </c>
+      <c r="C111" s="9">
+        <v>0.4765625</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>(26,1234,0.4765625),</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +3336,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2804,7 +4455,7 @@
       <c r="I34">
         <v>2</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="6">
         <v>53</v>
       </c>
       <c r="L34" t="str">
@@ -2840,7 +4491,7 @@
       <c r="I35">
         <v>3</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J35" s="6">
         <v>39</v>
       </c>
       <c r="L35" t="str">
@@ -2948,7 +4599,7 @@
       <c r="I38">
         <v>2</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="6">
         <v>43</v>
       </c>
       <c r="L38" t="str">
@@ -2984,7 +4635,7 @@
       <c r="I39">
         <v>3</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J39" s="6">
         <v>83</v>
       </c>
       <c r="L39" t="str">
@@ -3020,7 +4671,7 @@
       <c r="I40">
         <v>4</v>
       </c>
-      <c r="J40" s="7">
+      <c r="J40" s="6">
         <v>55</v>
       </c>
       <c r="L40" t="str">
@@ -3056,7 +4707,7 @@
       <c r="I41">
         <v>5</v>
       </c>
-      <c r="J41" s="7">
+      <c r="J41" s="6">
         <v>86</v>
       </c>
       <c r="L41" t="str">
@@ -3092,7 +4743,7 @@
       <c r="I42">
         <v>2</v>
       </c>
-      <c r="J42" s="7">
+      <c r="J42" s="6">
         <v>20</v>
       </c>
       <c r="L42" t="str">
@@ -3164,7 +4815,7 @@
       <c r="I44">
         <v>4</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="6">
         <v>80</v>
       </c>
       <c r="L44" t="str">
@@ -3200,7 +4851,7 @@
       <c r="I45">
         <v>5</v>
       </c>
-      <c r="J45" s="7">
+      <c r="J45" s="6">
         <v>69</v>
       </c>
       <c r="L45" t="str">
@@ -3272,7 +4923,7 @@
       <c r="I47">
         <v>3</v>
       </c>
-      <c r="J47" s="7">
+      <c r="J47" s="6">
         <v>66</v>
       </c>
       <c r="L47" t="str">
@@ -3308,7 +4959,7 @@
       <c r="I48">
         <v>4</v>
       </c>
-      <c r="J48" s="7">
+      <c r="J48" s="6">
         <v>21</v>
       </c>
       <c r="L48" t="str">
@@ -3344,7 +4995,7 @@
       <c r="I49">
         <v>5</v>
       </c>
-      <c r="J49" s="7">
+      <c r="J49" s="6">
         <v>47</v>
       </c>
       <c r="L49" t="str">
@@ -3380,7 +5031,7 @@
       <c r="I50">
         <v>6</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="6">
         <v>46</v>
       </c>
       <c r="L50" t="str">
@@ -3416,7 +5067,7 @@
       <c r="I51">
         <v>7</v>
       </c>
-      <c r="J51" s="7">
+      <c r="J51" s="6">
         <v>36</v>
       </c>
       <c r="L51" t="str">
@@ -3452,7 +5103,7 @@
       <c r="I52">
         <v>8</v>
       </c>
-      <c r="J52" s="7">
+      <c r="J52" s="6">
         <v>1</v>
       </c>
       <c r="L52" t="str">
@@ -3488,7 +5139,7 @@
       <c r="I53">
         <v>9</v>
       </c>
-      <c r="J53" s="7">
+      <c r="J53" s="6">
         <v>49</v>
       </c>
       <c r="L53" t="str">
@@ -3524,7 +5175,7 @@
       <c r="I54">
         <v>6</v>
       </c>
-      <c r="J54" s="7">
+      <c r="J54" s="6">
         <v>17</v>
       </c>
       <c r="L54" t="str">
@@ -3560,7 +5211,7 @@
       <c r="I55">
         <v>7</v>
       </c>
-      <c r="J55" s="7">
+      <c r="J55" s="6">
         <v>18</v>
       </c>
       <c r="L55" t="str">
@@ -3596,7 +5247,7 @@
       <c r="I56">
         <v>8</v>
       </c>
-      <c r="J56" s="7">
+      <c r="J56" s="6">
         <v>34</v>
       </c>
       <c r="L56" t="str">
@@ -3704,7 +5355,7 @@
       <c r="I59">
         <v>7</v>
       </c>
-      <c r="J59" s="7">
+      <c r="J59" s="6">
         <v>70</v>
       </c>
       <c r="L59" t="str">
@@ -3740,7 +5391,7 @@
       <c r="I60">
         <v>8</v>
       </c>
-      <c r="J60" s="7">
+      <c r="J60" s="6">
         <v>35</v>
       </c>
       <c r="L60" t="str">
@@ -3776,7 +5427,7 @@
       <c r="I61">
         <v>9</v>
       </c>
-      <c r="J61" s="7">
+      <c r="J61" s="6">
         <v>78</v>
       </c>
       <c r="L61" t="str">
@@ -3812,7 +5463,7 @@
       <c r="I62">
         <v>6</v>
       </c>
-      <c r="J62" s="7">
+      <c r="J62" s="6">
         <v>52</v>
       </c>
       <c r="L62" t="str">
@@ -3848,7 +5499,7 @@
       <c r="I63">
         <v>7</v>
       </c>
-      <c r="J63" s="7">
+      <c r="J63" s="6">
         <v>59</v>
       </c>
       <c r="L63" t="str">
@@ -3884,7 +5535,7 @@
       <c r="I64">
         <v>8</v>
       </c>
-      <c r="J64" s="7">
+      <c r="J64" s="6">
         <v>82</v>
       </c>
       <c r="L64" t="str">
@@ -3956,7 +5607,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3968,10 +5619,10 @@
       <c r="E1" t="s">
         <v>274</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -3987,10 +5638,10 @@
         <f t="shared" ref="E2:E33" si="0">"("&amp;A2&amp;",'"&amp;B2&amp;"',"&amp;C2&amp;")"&amp;IF(LEN(A3)&gt;0,",","")</f>
         <v>(1,'Aaron Rodgers',1),</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -4006,10 +5657,10 @@
         <f t="shared" si="0"/>
         <v>(2,'Andy Dalton',1),</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -4025,10 +5676,10 @@
         <f t="shared" si="0"/>
         <v>(3,'Baker Mayfield',1),</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -4044,9 +5695,9 @@
         <f t="shared" si="0"/>
         <v>(4,'Ben Roethlisberger',0),</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -4062,9 +5713,9 @@
         <f t="shared" si="0"/>
         <v>(5,'Blaine Gabbert',1),</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -4080,10 +5731,10 @@
         <f t="shared" si="0"/>
         <v>(6,'Brandon Allen',1),</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -4099,10 +5750,10 @@
         <f t="shared" si="0"/>
         <v>(7,'Brett Rypien',1),</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -4118,10 +5769,10 @@
         <f t="shared" si="0"/>
         <v>(8,'Brian Hoyer',1),</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -4137,10 +5788,10 @@
         <f t="shared" si="0"/>
         <v>(9,'Bryce Perkins',1),</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -4156,10 +5807,10 @@
         <f t="shared" si="0"/>
         <v>(10,'Cam Newton',1),</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -4175,10 +5826,10 @@
         <f t="shared" si="0"/>
         <v>(11,'Carson Wentz',1),</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -4194,10 +5845,10 @@
         <f t="shared" si="0"/>
         <v>(12,'Case Keenum',1),</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -4213,10 +5864,10 @@
         <f t="shared" si="0"/>
         <v>(13,'Chad Henne',1),</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -4232,10 +5883,10 @@
         <f t="shared" si="0"/>
         <v>(14,'Chase Daniel',1),</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -4251,10 +5902,10 @@
         <f t="shared" si="0"/>
         <v>(15,'Colt McCoy',1),</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -4270,10 +5921,10 @@
         <f t="shared" si="0"/>
         <v>(16,'Cooper Rush',1),</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -4289,10 +5940,10 @@
         <f t="shared" si="0"/>
         <v>(17,'Dak Prescott',1),</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -4308,10 +5959,10 @@
         <f t="shared" si="0"/>
         <v>(18,'Daniel Jones',1),</v>
       </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -4327,10 +5978,10 @@
         <f t="shared" si="0"/>
         <v>(19,'David Blough',1),</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -4346,10 +5997,10 @@
         <f t="shared" si="0"/>
         <v>(20,'Davis Mills',1),</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -4365,10 +6016,10 @@
         <f t="shared" si="0"/>
         <v>(21,'Derek Carr',1),</v>
       </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -4384,10 +6035,10 @@
         <f t="shared" si="0"/>
         <v>(22,'Deshaun Watson',1),</v>
       </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -4403,10 +6054,10 @@
         <f t="shared" si="0"/>
         <v>(23,'Drew Lock',1),</v>
       </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -4422,10 +6073,10 @@
         <f t="shared" si="0"/>
         <v>(24,'Dwayne Haskins',0),</v>
       </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -4441,10 +6092,10 @@
         <f t="shared" si="0"/>
         <v>(25,'Easton Stick',1),</v>
       </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -4460,10 +6111,10 @@
         <f t="shared" si="0"/>
         <v>(26,'Feleipe Franks',1),</v>
       </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -4479,10 +6130,10 @@
         <f t="shared" si="0"/>
         <v>(27,'Gardner Minshew',1),</v>
       </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -4498,10 +6149,10 @@
         <f t="shared" si="0"/>
         <v>(28,'Garrett Gilbert',1),</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -4517,10 +6168,10 @@
         <f t="shared" si="0"/>
         <v>(29,'Geno Smith',1),</v>
       </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -4536,10 +6187,10 @@
         <f t="shared" si="0"/>
         <v>(30,'Ian Book',1),</v>
       </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -4555,10 +6206,10 @@
         <f t="shared" si="0"/>
         <v>(31,'Jacob Eason',1),</v>
       </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -4574,10 +6225,10 @@
         <f t="shared" si="0"/>
         <v>(32,'Jacoby Brissett',1),</v>
       </c>
-      <c r="I33" s="9"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -4593,10 +6244,10 @@
         <f t="shared" ref="E34:E65" si="1">"("&amp;A34&amp;",'"&amp;B34&amp;"',"&amp;C34&amp;")"&amp;IF(LEN(A35)&gt;0,",","")</f>
         <v>(33,'Jake Fromm',1),</v>
       </c>
-      <c r="I34" s="9"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -4612,10 +6263,10 @@
         <f t="shared" si="1"/>
         <v>(34,'Jalen Hurts',1),</v>
       </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -4631,10 +6282,10 @@
         <f t="shared" si="1"/>
         <v>(35,'Jameis Winston',1),</v>
       </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -4650,10 +6301,10 @@
         <f t="shared" si="1"/>
         <v>(36,'Jared Goff',1),</v>
       </c>
-      <c r="I37" s="9"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -4669,10 +6320,10 @@
         <f t="shared" si="1"/>
         <v>(37,'Jarrett Stidham',1),</v>
       </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
@@ -4688,10 +6339,10 @@
         <f t="shared" si="1"/>
         <v>(38,'Jimmy Garoppolo',1),</v>
       </c>
-      <c r="I39" s="9"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -4707,10 +6358,10 @@
         <f t="shared" si="1"/>
         <v>(39,'Joe Burrow',1),</v>
       </c>
-      <c r="I40" s="9"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -4726,10 +6377,10 @@
         <f t="shared" si="1"/>
         <v>(40,'Joe Flacco',1),</v>
       </c>
-      <c r="I41" s="9"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -4745,10 +6396,10 @@
         <f t="shared" si="1"/>
         <v>(41,'John Wolford',1),</v>
       </c>
-      <c r="I42" s="9"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -4764,10 +6415,10 @@
         <f t="shared" si="1"/>
         <v>(42,'Jordan Love',1),</v>
       </c>
-      <c r="I43" s="9"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -4783,10 +6434,10 @@
         <f t="shared" si="1"/>
         <v>(43,'Josh Allen',1),</v>
       </c>
-      <c r="I44" s="9"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -4802,10 +6453,10 @@
         <f t="shared" si="1"/>
         <v>(44,'Josh Johnson',1),</v>
       </c>
-      <c r="I45" s="9"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -4821,10 +6472,10 @@
         <f t="shared" si="1"/>
         <v>(45,'Josh Rosen',1),</v>
       </c>
-      <c r="I46" s="9"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -4840,10 +6491,10 @@
         <f t="shared" si="1"/>
         <v>(46,'Justin Fields',1),</v>
       </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -4859,10 +6510,10 @@
         <f t="shared" si="1"/>
         <v>(47,'Justin Herbert',1),</v>
       </c>
-      <c r="I48" s="9"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -4878,10 +6529,10 @@
         <f t="shared" si="1"/>
         <v>(48,'Kellen Mond',1),</v>
       </c>
-      <c r="I49" s="9"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -4897,10 +6548,10 @@
         <f t="shared" si="1"/>
         <v>(49,'Kirk Cousins',1),</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -4916,10 +6567,10 @@
         <f t="shared" si="1"/>
         <v>(50,'Kyle Allen',1),</v>
       </c>
-      <c r="I51" s="9"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -4935,10 +6586,10 @@
         <f t="shared" si="1"/>
         <v>(51,'Kyle Trask',1),</v>
       </c>
-      <c r="I52" s="9"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -4954,10 +6605,10 @@
         <f t="shared" si="1"/>
         <v>(52,'Kyler Murray',1),</v>
       </c>
-      <c r="I53" s="9"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -4973,10 +6624,10 @@
         <f t="shared" si="1"/>
         <v>(53,'Lamar Jackson',1),</v>
       </c>
-      <c r="I54" s="9"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -4992,10 +6643,10 @@
         <f t="shared" si="1"/>
         <v>(54,'Logan Woodside',1),</v>
       </c>
-      <c r="I55" s="9"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -5011,10 +6662,10 @@
         <f t="shared" si="1"/>
         <v>(55,'Mac Jones',1),</v>
       </c>
-      <c r="I56" s="9"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -5030,10 +6681,10 @@
         <f t="shared" si="1"/>
         <v>(56,'Marcus Mariota',1),</v>
       </c>
-      <c r="I57" s="9"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -5049,10 +6700,10 @@
         <f t="shared" si="1"/>
         <v>(57,'Mason Rudolph',1),</v>
       </c>
-      <c r="I58" s="9"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -5068,10 +6719,10 @@
         <f t="shared" si="1"/>
         <v>(58,'Matt Ryan',1),</v>
       </c>
-      <c r="I59" s="9"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -5087,10 +6738,10 @@
         <f t="shared" si="1"/>
         <v>(59,'Matthew Stafford',1),</v>
       </c>
-      <c r="I60" s="9"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -5106,10 +6757,10 @@
         <f t="shared" si="1"/>
         <v>(60,'Mike Glennon',1),</v>
       </c>
-      <c r="I61" s="9"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -5125,10 +6776,10 @@
         <f t="shared" si="1"/>
         <v>(61,'Mike White',1),</v>
       </c>
-      <c r="I62" s="9"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -5144,10 +6795,10 @@
         <f t="shared" si="1"/>
         <v>(62,'Mitchell Trubisky',1),</v>
       </c>
-      <c r="I63" s="9"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
-      <c r="L63" s="6"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -5163,10 +6814,10 @@
         <f t="shared" si="1"/>
         <v>(63,'Nick Foles',1),</v>
       </c>
-      <c r="I64" s="9"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -5182,10 +6833,10 @@
         <f t="shared" si="1"/>
         <v>(64,'Nick Mullens',1),</v>
       </c>
-      <c r="I65" s="9"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -5201,10 +6852,10 @@
         <f t="shared" ref="E66:E94" si="2">"("&amp;A66&amp;",'"&amp;B66&amp;"',"&amp;C66&amp;")"&amp;IF(LEN(A67)&gt;0,",","")</f>
         <v>(65,'PJ Walker',1),</v>
       </c>
-      <c r="I66" s="9"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -5220,10 +6871,10 @@
         <f t="shared" si="2"/>
         <v>(66,'Patrick Mahomes',1),</v>
       </c>
-      <c r="I67" s="9"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
-      <c r="L67" s="6"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -5239,10 +6890,10 @@
         <f t="shared" si="2"/>
         <v>(67,'Reid Sinnett',1),</v>
       </c>
-      <c r="I68" s="9"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
@@ -5258,10 +6909,10 @@
         <f t="shared" si="2"/>
         <v>(68,'Russell Wilson',1),</v>
       </c>
-      <c r="I69" s="9"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
@@ -5277,10 +6928,10 @@
         <f t="shared" si="2"/>
         <v>(69,'Ryan Tannehill',1),</v>
       </c>
-      <c r="I70" s="9"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
@@ -5296,10 +6947,10 @@
         <f t="shared" si="2"/>
         <v>(70,'Sam Darnold',1),</v>
       </c>
-      <c r="I71" s="9"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
@@ -5315,10 +6966,10 @@
         <f t="shared" si="2"/>
         <v>(71,'Sam Ehlinger',1),</v>
       </c>
-      <c r="I72" s="9"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
@@ -5334,10 +6985,10 @@
         <f t="shared" si="2"/>
         <v>(72,'Sean Mannion',1),</v>
       </c>
-      <c r="I73" s="9"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
@@ -5353,10 +7004,10 @@
         <f t="shared" si="2"/>
         <v>(73,'Shane Buechele',1),</v>
       </c>
-      <c r="I74" s="9"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
@@ -5372,10 +7023,10 @@
         <f t="shared" si="2"/>
         <v>(74,'Taylor Heinicke',1),</v>
       </c>
-      <c r="I75" s="9"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -5391,10 +7042,10 @@
         <f t="shared" si="2"/>
         <v>(75,'Taysom Hill',1),</v>
       </c>
-      <c r="I76" s="9"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
@@ -5410,10 +7061,10 @@
         <f t="shared" si="2"/>
         <v>(76,'Teddy Bridgewater',1),</v>
       </c>
-      <c r="I77" s="9"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -5429,10 +7080,10 @@
         <f t="shared" si="2"/>
         <v>(77,'Tim Boyle',1),</v>
       </c>
-      <c r="I78" s="9"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
@@ -5448,10 +7099,10 @@
         <f t="shared" si="2"/>
         <v>(78,'Tom Brady',1),</v>
       </c>
-      <c r="I79" s="9"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
@@ -5467,10 +7118,10 @@
         <f t="shared" si="2"/>
         <v>(79,'Trace McSorley',1),</v>
       </c>
-      <c r="I80" s="9"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
@@ -5486,10 +7137,10 @@
         <f t="shared" si="2"/>
         <v>(80,'Trevor Lawrence',1),</v>
       </c>
-      <c r="I81" s="9"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
@@ -5505,10 +7156,10 @@
         <f t="shared" si="2"/>
         <v>(81,'Trevor Siemian',1),</v>
       </c>
-      <c r="I82" s="9"/>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
-      <c r="L82" s="6"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
@@ -5524,10 +7175,10 @@
         <f t="shared" si="2"/>
         <v>(82,'Trey Lance',1),</v>
       </c>
-      <c r="I83" s="9"/>
-      <c r="J83" s="6"/>
-      <c r="K83" s="6"/>
-      <c r="L83" s="6"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
@@ -5543,10 +7194,10 @@
         <f t="shared" si="2"/>
         <v>(83,'Tua Tagovailoa',1),</v>
       </c>
-      <c r="I84" s="9"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
-      <c r="L84" s="6"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
@@ -5562,10 +7213,10 @@
         <f t="shared" si="2"/>
         <v>(84,'Tyler Huntley',1),</v>
       </c>
-      <c r="I85" s="9"/>
-      <c r="J85" s="6"/>
-      <c r="K85" s="6"/>
-      <c r="L85" s="6"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86">
@@ -5581,10 +7232,10 @@
         <f t="shared" si="2"/>
         <v>(85,'Tyrod Taylor',1),</v>
       </c>
-      <c r="I86" s="9"/>
-      <c r="J86" s="6"/>
-      <c r="K86" s="6"/>
-      <c r="L86" s="6"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87">
@@ -5600,10 +7251,10 @@
         <f t="shared" si="2"/>
         <v>(86,'Zach Wilson',1),</v>
       </c>
-      <c r="I87" s="9"/>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
@@ -5619,10 +7270,10 @@
         <f t="shared" si="2"/>
         <v>(87,'Bailey Zappe',1),</v>
       </c>
-      <c r="I88" s="9"/>
-      <c r="J88" s="6"/>
-      <c r="K88" s="6"/>
-      <c r="L88" s="6"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
@@ -5638,10 +7289,10 @@
         <f t="shared" si="2"/>
         <v>(88,'Carson Strong',1),</v>
       </c>
-      <c r="I89" s="9"/>
-      <c r="J89" s="6"/>
-      <c r="K89" s="6"/>
-      <c r="L89" s="6"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
@@ -5657,10 +7308,10 @@
         <f t="shared" si="2"/>
         <v>(89,'Desmond Ridder',1),</v>
       </c>
-      <c r="I90" s="9"/>
-      <c r="J90" s="6"/>
-      <c r="K90" s="6"/>
-      <c r="L90" s="6"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91">
@@ -5676,10 +7327,10 @@
         <f t="shared" si="2"/>
         <v>(90,'Kenny Pickett',1),</v>
       </c>
-      <c r="I91" s="9"/>
-      <c r="J91" s="6"/>
-      <c r="K91" s="6"/>
-      <c r="L91" s="6"/>
+      <c r="I91" s="8"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92">
@@ -5695,10 +7346,10 @@
         <f t="shared" si="2"/>
         <v>(91,'Malik Willis',1),</v>
       </c>
-      <c r="I92" s="9"/>
-      <c r="J92" s="6"/>
-      <c r="K92" s="6"/>
-      <c r="L92" s="6"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
@@ -5714,10 +7365,10 @@
         <f t="shared" si="2"/>
         <v>(92,'Matt Corral',1),</v>
       </c>
-      <c r="I93" s="9"/>
-      <c r="J93" s="6"/>
-      <c r="K93" s="6"/>
-      <c r="L93" s="6"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
@@ -5733,10 +7384,10 @@
         <f t="shared" si="2"/>
         <v>(93,'Sam Howell',1),</v>
       </c>
-      <c r="I94" s="9"/>
-      <c r="J94" s="6"/>
-      <c r="K94" s="6"/>
-      <c r="L94" s="6"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95">
@@ -5752,10 +7403,10 @@
         <f t="shared" ref="E95:E105" si="3">"("&amp;A95&amp;",'"&amp;B95&amp;"',"&amp;C95&amp;")"&amp;IF(LEN(A96)&gt;0,",","")</f>
         <v>(94,'Bryce Young',1),</v>
       </c>
-      <c r="I95" s="9"/>
-      <c r="J95" s="6"/>
-      <c r="K95" s="6"/>
-      <c r="L95" s="6"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
@@ -6096,7 +7747,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -6104,10 +7755,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>232</v>
       </c>
       <c r="D2" t="s">
@@ -6115,10 +7766,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>233</v>
       </c>
       <c r="D3" t="s">
@@ -6126,10 +7777,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>234</v>
       </c>
       <c r="D4" t="s">
@@ -6243,7 +7894,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -6326,7 +7977,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -6605,7 +8256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F502399-C795-4D5E-88DC-92C8B5181153}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -6618,7 +8269,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>235</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
Franchise added and register page re-designed, register request needs testing, including fav franchise setting
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681E777B-A1B1-4FC2-8BC8-210194DF9CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FB85FE-CCB6-4557-BEAC-CC6BC8F758F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="ScoringSettings" sheetId="10" r:id="rId12"/>
     <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
     <sheet name="UserScores" sheetId="12" r:id="rId14"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId15"/>
+    <sheet name="Franchises" sheetId="18" r:id="rId15"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$C$87</definedName>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="288">
   <si>
     <t>TeamID</t>
   </si>
@@ -926,6 +927,18 @@
   </si>
   <si>
     <t xml:space="preserve">INSERT INTO UserScores (UserID,PredictionPeriodID,Score) VALUES </t>
+  </si>
+  <si>
+    <t>FranchiseID</t>
+  </si>
+  <si>
+    <t>Location2022</t>
+  </si>
+  <si>
+    <t>Nickname2022</t>
+  </si>
+  <si>
+    <t>INSERT INTO Franchises (FranchiseID, Location2022, Nickname2022) VALUES</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1626,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C905B6-0F24-42C4-A0E7-3FA0C74BEC6D}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D111"/>
     </sheetView>
   </sheetViews>
@@ -3305,6 +3318,521 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B34627-8194-453E-A9E5-FAABA9941246}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"'),"</f>
+        <v>(1,'Baltimore','Ravens'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E33" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"'),"</f>
+        <v>(2,'Cincinnati','Bengals'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'Cleveland','Browns'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,'Pittsburgh','Steelers'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,'Buffalo','Bills'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,'Miami','Dolphins'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,'New England','Patriots'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,'New York','Jets'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,'Houston','Texans'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,'Indianapolis','Colts'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,'Jacksonville','Jaguars'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,'Tennessee','Titans'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,'Denver','Broncos'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,'Kansas City','Chiefs'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,'Las Vegas','Raiders'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,'Los Angeles','Chargers'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,'Chicago','Bears'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,'Detroit','Lions'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,'Green Bay','Packers'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,'Minnesota','Vikings'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,'Dallas','Cowboys'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,'New York','Giants'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,'Philadelphia','Eagles'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,'Washington','Commanders'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>(25,'Atlanta','Falcons'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>(26,'Carolina','Panthers'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>(27,'New Orleans','Saints'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>(28,'Tampa Bay','Buccaneers'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>(29,'Arizona','Cardinals'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>(30,'Los Angeles','Rams'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>(31,'San Francisco','49ers'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>(32,'Seattle','Seahawks'),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3320,8 +3848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3365,6 +3893,9 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>276</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="L1" t="str">
         <f>"INSERT INTO the_qb_carousel.teams ("&amp;_xlfn.TEXTJOIN(",",FALSE,A1:J1)&amp;") VALUES"</f>

</xml_diff>

<commit_message>
Email models set up
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FB85FE-CCB6-4557-BEAC-CC6BC8F758F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1026308-41B5-4C6F-A232-8878E2C078CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <sheet name="PrivateLeagueMembers" sheetId="11" r:id="rId13"/>
     <sheet name="UserScores" sheetId="12" r:id="rId14"/>
     <sheet name="Franchises" sheetId="18" r:id="rId15"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId16"/>
+    <sheet name="EmailSubscriptions" sheetId="19" r:id="rId16"/>
+    <sheet name="EmailSubscriptionTypes" sheetId="20" r:id="rId17"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$C$87</definedName>
@@ -75,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="296">
   <si>
     <t>TeamID</t>
   </si>
@@ -939,6 +941,30 @@
   </si>
   <si>
     <t>INSERT INTO Franchises (FranchiseID, Location2022, Nickname2022) VALUES</t>
+  </si>
+  <si>
+    <t>EmailSubscriptionTypeID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>EmailSubscriptionType</t>
+  </si>
+  <si>
+    <t>EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODOPEN</t>
+  </si>
+  <si>
+    <t>EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODCLOSE</t>
+  </si>
+  <si>
+    <t>Email sent out just after the prediction period has opened</t>
+  </si>
+  <si>
+    <t>Email sent out about a week before the prediction period closes</t>
+  </si>
+  <si>
+    <t>INSERT INTO EmailSubscriptionTypes (EmailSubscriptionTypeID,EmailSubscriptionType,Description) VALUES</t>
   </si>
 </sst>
 </file>
@@ -3833,6 +3859,102 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC6C2B3-0879-4D8D-928D-DD2F288018F7}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789449E2-1E71-4639-A31F-FEE451B9A1CF}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"'),"</f>
+        <v>(1,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"'),"</f>
+        <v>(2,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes'),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3848,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working on building emails, current estyes code may be dodgy though
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1026308-41B5-4C6F-A232-8878E2C078CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50713C6E-12E5-4CD6-98DD-C1F7098C9076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="299">
   <si>
     <t>TeamID</t>
   </si>
@@ -964,7 +964,16 @@
     <t>Email sent out about a week before the prediction period closes</t>
   </si>
   <si>
-    <t>INSERT INTO EmailSubscriptionTypes (EmailSubscriptionTypeID,EmailSubscriptionType,Description) VALUES</t>
+    <t>EmailSubscriptionTypeTidy</t>
+  </si>
+  <si>
+    <t>Prediction Period Open</t>
+  </si>
+  <si>
+    <t>Prediction Period Close</t>
+  </si>
+  <si>
+    <t>INSERT INTO EmailSubscriptionTypes (EmailSubscriptionTypeID,EmailSubscriptionType,Description,EmailSubscriptionTypeTidy) VALUES</t>
   </si>
 </sst>
 </file>
@@ -3892,10 +3901,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789449E2-1E71-4639-A31F-FEE451B9A1CF}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3903,9 +3912,10 @@
     <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>288</v>
       </c>
@@ -3918,8 +3928,11 @@
       <c r="D1" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3929,12 +3942,15 @@
       <c r="C2" t="s">
         <v>293</v>
       </c>
-      <c r="D2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"'),"</f>
-        <v>(1,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened'),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"'),"</f>
+        <v>(1,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened','Prediction Period Open'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3944,9 +3960,12 @@
       <c r="C3" t="s">
         <v>294</v>
       </c>
-      <c r="D3" t="str">
-        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"'),"</f>
-        <v>(2,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes'),</v>
+      <c r="D3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" t="str">
+        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"'),"</f>
+        <v>(2,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes','Prediction Period Close'),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created email history table, onto bulk sending emails
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50713C6E-12E5-4CD6-98DD-C1F7098C9076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98578060-CCF3-4410-815C-14791AB733EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -29,8 +29,9 @@
     <sheet name="UserScores" sheetId="12" r:id="rId14"/>
     <sheet name="Franchises" sheetId="18" r:id="rId15"/>
     <sheet name="EmailSubscriptions" sheetId="19" r:id="rId16"/>
-    <sheet name="EmailSubscriptionTypes" sheetId="20" r:id="rId17"/>
-    <sheet name="SQL Commands" sheetId="13" r:id="rId18"/>
+    <sheet name="EmailTypes" sheetId="20" r:id="rId17"/>
+    <sheet name="Dates" sheetId="21" r:id="rId18"/>
+    <sheet name="SQL Commands" sheetId="13" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Players!$A$1:$C$87</definedName>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="324">
   <si>
     <t>TeamID</t>
   </si>
@@ -949,31 +950,106 @@
     <t>Value</t>
   </si>
   <si>
-    <t>EmailSubscriptionType</t>
-  </si>
-  <si>
-    <t>EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODOPEN</t>
-  </si>
-  <si>
-    <t>EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODCLOSE</t>
-  </si>
-  <si>
     <t>Email sent out just after the prediction period has opened</t>
   </si>
   <si>
     <t>Email sent out about a week before the prediction period closes</t>
   </si>
   <si>
-    <t>EmailSubscriptionTypeTidy</t>
-  </si>
-  <si>
     <t>Prediction Period Open</t>
   </si>
   <si>
     <t>Prediction Period Close</t>
   </si>
   <si>
-    <t>INSERT INTO EmailSubscriptionTypes (EmailSubscriptionTypeID,EmailSubscriptionType,Description,EmailSubscriptionTypeTidy) VALUES</t>
+    <t>EmaiTypeID</t>
+  </si>
+  <si>
+    <t>EmailType</t>
+  </si>
+  <si>
+    <t>EmailTypeTidy</t>
+  </si>
+  <si>
+    <t>IsSubscription</t>
+  </si>
+  <si>
+    <t>EMAILTYPE_PREDICTIONPERIODOPEN</t>
+  </si>
+  <si>
+    <t>EMAILTYPE_PREDICTIONPERIODCLOSE</t>
+  </si>
+  <si>
+    <t>EMAILTYPE_EMAILVERIFICATION</t>
+  </si>
+  <si>
+    <t>Email to verify user's email after registration</t>
+  </si>
+  <si>
+    <t>Email Verification</t>
+  </si>
+  <si>
+    <t>INSERT INTO EmailTypes (EmailTypeID,EmailType,Description,EmailTypeTidy,IsSubscription) VALUES</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>ConfirmationTokens</t>
+  </si>
+  <si>
+    <t>SQL DT</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>PeriodPredictions</t>
+  </si>
+  <si>
+    <t>PredictionDateTimeUTC</t>
+  </si>
+  <si>
+    <t>Java DT</t>
+  </si>
+  <si>
+    <t>RefreshTokens</t>
+  </si>
+  <si>
+    <t>LastUsageDateTimeUTC</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>ZonedDateTime</t>
+  </si>
+  <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t>UserCreateDateTimeUTC</t>
+  </si>
+  <si>
+    <t>CreatedDateTimeUTC</t>
+  </si>
+  <si>
+    <t>EmailHistory</t>
+  </si>
+  <si>
+    <t>RowCreatedDateTimeUTC</t>
+  </si>
+  <si>
+    <t>EmailSentDateTimeUTC</t>
   </si>
 </sst>
 </file>
@@ -3901,10 +3977,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789449E2-1E71-4639-A31F-FEE451B9A1CF}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3913,59 +3989,90 @@
     <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>291</v>
-      </c>
       <c r="C2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"'),"</f>
-        <v>(1,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened','Prediction Period Open'),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;"),"</f>
+        <v>(1,'EMAILTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened','Prediction Period Open',1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E3" t="str">
-        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"'),"</f>
-        <v>(2,'EMAILSUBSCRIPTIONTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes','Prediction Period Close'),</v>
+        <v>293</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;"),"</f>
+        <v>(2,'EMAILTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes','Prediction Period Close',1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"("&amp;A4&amp;",'"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"',"&amp;E4&amp;"),"</f>
+        <v>(3,'EMAILTYPE_EMAILVERIFICATION','Email to verify user's email after registration','Email Verification',0),</v>
       </c>
     </row>
   </sheetData>
@@ -3974,6 +4081,143 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BF2485-3463-40E7-9672-C2FAD607F623}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D7" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>321</v>
+      </c>
+      <c r="C8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C29077-A30D-4782-9EC4-DB0B084B9BA7}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Password reset now possible
</commit_message>
<xml_diff>
--- a/Other files/Tables.xlsx
+++ b/Other files/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98578060-CCF3-4410-815C-14791AB733EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029FF015-1077-4041-B594-F9D6577D1310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="833" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDsInfo" sheetId="9" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="327">
   <si>
     <t>TeamID</t>
   </si>
@@ -1050,6 +1050,15 @@
   </si>
   <si>
     <t>EmailSentDateTimeUTC</t>
+  </si>
+  <si>
+    <t>EMAILTYPE_PASSWORDRESET</t>
+  </si>
+  <si>
+    <t>Email sent out to reset user's email</t>
+  </si>
+  <si>
+    <t>Password Reset</t>
   </si>
 </sst>
 </file>
@@ -3977,15 +3986,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789449E2-1E71-4639-A31F-FEE451B9A1CF}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
@@ -4029,7 +4038,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;"),"</f>
+        <f>"("&amp;A2&amp;",'"&amp;B2&amp;"','"&amp;SUBSTITUTE(C2,"'","''")&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;"),"</f>
         <v>(1,'EMAILTYPE_PREDICTIONPERIODOPEN','Email sent out just after the prediction period has opened','Prediction Period Open',1),</v>
       </c>
     </row>
@@ -4050,7 +4059,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f>"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;"),"</f>
+        <f t="shared" ref="F3:F5" si="0">"("&amp;A3&amp;",'"&amp;B3&amp;"','"&amp;SUBSTITUTE(C3,"'","''")&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;"),"</f>
         <v>(2,'EMAILTYPE_PREDICTIONPERIODCLOSE','Email sent out about a week before the prediction period closes','Prediction Period Close',1),</v>
       </c>
     </row>
@@ -4071,8 +4080,29 @@
         <v>0</v>
       </c>
       <c r="F4" t="str">
-        <f>"("&amp;A4&amp;",'"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"',"&amp;E4&amp;"),"</f>
-        <v>(3,'EMAILTYPE_EMAILVERIFICATION','Email to verify user's email after registration','Email Verification',0),</v>
+        <f t="shared" si="0"/>
+        <v>(3,'EMAILTYPE_EMAILVERIFICATION','Email to verify user''s email after registration','Email Verification',0),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,'EMAILTYPE_PASSWORDRESET','Email sent out to reset user''s email','Password Reset',0),</v>
       </c>
     </row>
   </sheetData>
@@ -4084,7 +4114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BF2485-3463-40E7-9672-C2FAD607F623}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>